<commit_message>
Published state of ETDataset on 26 October 2017
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/bio_oil.carrier.xlsx
+++ b/carriers_source_analyses/bio_oil.carrier.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorinevandervlies/Projects/etdataset/carriers_source_analyses/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16100" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="44660" yWindow="-7880" windowWidth="28800" windowHeight="16100" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -32,8 +37,11 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -330,9 +338,6 @@
   </si>
   <si>
     <t>Document</t>
-  </si>
-  <si>
-    <t>This sheet summarizes all carrier attributes formatted in the way they are used by the Energy Transition Model. This sheet contains only pure carrier values. For some countries and carriers Fuel Chain Emissions are defined (only for NL); if so these FCE are documented in a separate sheet (e.g. nl_fce). Use the Excel formulas to find the original data and sources for these numbers.</t>
   </si>
   <si>
     <t>potential_co2_conversion_per_mj</t>
@@ -486,6 +491,9 @@
   <si>
     <t>definition biodiesels and other liquid buifuels</t>
   </si>
+  <si>
+    <t xml:space="preserve">This sheet summarizes all carrier attributes formatted in the way they are used by the Energy Transition Model. This sheet contains only pure carrier values. For some countries and carriers Fuel Chain Emissions are defined (only for NL); if so these FCE are documented in a separate sheet (e.g. nl_fce). Use the Excel formulas to find the original data and sources for these numbers. The carrier analysis can be imported on ETSource by running the following rake task: rake import:carrier CARRIER="carrier name" (eg rake import:carrier CARRIER=crude_oil) </t>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +505,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -683,11 +691,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1657,40 +1660,41 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1718,11 +1722,10 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="348">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2076,80 +2079,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>3949700</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="export_data" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
-                </a:rPr>
-                <a:t>Update carrier attributes on ETSource</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2638,7 +2576,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -2751,12 +2689,13 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
       <sheetName val="carrier_manager.xlsm"/>
+      <sheetName val="carrier_manager"/>
     </sheetNames>
     <definedNames>
       <definedName name="update_attributes"/>
@@ -2765,6 +2704,7 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3097,33 +3037,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="44.125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="2.125" style="21" customWidth="1"/>
-    <col min="5" max="16384" width="10.625" style="21"/>
+    <col min="1" max="1" width="3.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1">
+    <row r="1" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:4" ht="20">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="28"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>95</v>
@@ -3132,7 +3072,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="10" t="s">
         <v>13</v>
@@ -3141,7 +3081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -3150,17 +3090,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="79" t="s">
         <v>14</v>
@@ -3168,13 +3108,13 @@
       <c r="C9" s="80"/>
       <c r="D9" s="124"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="81"/>
       <c r="C10" s="82"/>
       <c r="D10" s="125"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="81" t="s">
         <v>15</v>
@@ -3184,7 +3124,7 @@
       </c>
       <c r="D11" s="125"/>
     </row>
-    <row r="12" spans="1:4" ht="16" thickBot="1">
+    <row r="12" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="81"/>
       <c r="C12" s="18" t="s">
@@ -3192,7 +3132,7 @@
       </c>
       <c r="D12" s="125"/>
     </row>
-    <row r="13" spans="1:4" ht="16" thickBot="1">
+    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="81"/>
       <c r="C13" s="84" t="s">
@@ -3200,7 +3140,7 @@
       </c>
       <c r="D13" s="125"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="81"/>
       <c r="C14" s="82" t="s">
@@ -3208,13 +3148,13 @@
       </c>
       <c r="D14" s="125"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="81"/>
       <c r="C15" s="82"/>
       <c r="D15" s="125"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="81" t="s">
         <v>20</v>
@@ -3224,7 +3164,7 @@
       </c>
       <c r="D16" s="125"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="81"/>
       <c r="C17" s="86" t="s">
@@ -3232,7 +3172,7 @@
       </c>
       <c r="D17" s="125"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="81"/>
       <c r="C18" s="87" t="s">
@@ -3240,7 +3180,7 @@
       </c>
       <c r="D18" s="125"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="81"/>
       <c r="C19" s="88" t="s">
@@ -3248,7 +3188,7 @@
       </c>
       <c r="D19" s="125"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="89"/>
       <c r="C20" s="90" t="s">
@@ -3256,7 +3196,7 @@
       </c>
       <c r="D20" s="125"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="89"/>
       <c r="C21" s="91" t="s">
@@ -3264,7 +3204,7 @@
       </c>
       <c r="D21" s="125"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="89"/>
       <c r="C22" s="92" t="s">
@@ -3272,14 +3212,14 @@
       </c>
       <c r="D22" s="125"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="89"/>
       <c r="C23" s="93" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="125"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="126"/>
       <c r="C24" s="127"/>
       <c r="D24" s="128"/>
@@ -3287,76 +3227,71 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="B1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="35" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="35" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="46" style="35" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.375" style="35" customWidth="1"/>
-    <col min="6" max="6" width="4.625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" style="35" customWidth="1"/>
     <col min="7" max="7" width="45" style="35" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="35" customWidth="1"/>
-    <col min="9" max="9" width="51.5" style="35" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="35" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="35"/>
+    <col min="8" max="8" width="5.140625" style="35" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" style="35" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="35" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
     </row>
-    <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="162" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+    <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="163" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
     </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="165"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="167"/>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="168"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
     </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="168"/>
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="170"/>
+    <row r="4" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="169"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
     </row>
-    <row r="5" spans="2:11" ht="16" thickBot="1">
+    <row r="5" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D5" s="33"/>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="36"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -3367,7 +3302,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="37"/>
     </row>
-    <row r="7" spans="2:11" s="42" customFormat="1" ht="18">
+    <row r="7" spans="2:11" s="42" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="94"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -3388,7 +3323,7 @@
       </c>
       <c r="J7" s="96"/>
     </row>
-    <row r="8" spans="2:11" s="42" customFormat="1" ht="18">
+    <row r="8" spans="2:11" s="42" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
       <c r="C8" s="18"/>
       <c r="D8" s="31"/>
@@ -3399,7 +3334,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="43"/>
     </row>
-    <row r="9" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="9" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23"/>
       <c r="C9" s="123" t="s">
         <v>92</v>
@@ -3412,7 +3347,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="43"/>
     </row>
-    <row r="10" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="10" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23"/>
       <c r="C10" s="102" t="s">
         <v>36</v>
@@ -3434,7 +3369,7 @@
       </c>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="11" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
       <c r="C11" s="104" t="s">
         <v>37</v>
@@ -3454,7 +3389,7 @@
       </c>
       <c r="J11" s="43"/>
     </row>
-    <row r="12" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="12" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23"/>
       <c r="C12" s="122" t="s">
         <v>93</v>
@@ -3474,7 +3409,7 @@
       </c>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="13" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23"/>
       <c r="C13" s="122" t="s">
         <v>38</v>
@@ -3488,7 +3423,7 @@
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="131" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="105" t="s">
@@ -3496,10 +3431,10 @@
       </c>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="2:11" s="42" customFormat="1" ht="19" thickBot="1">
+    <row r="14" spans="2:11" s="42" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23"/>
       <c r="C14" s="129" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>43</v>
@@ -3510,15 +3445,15 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="131" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="156" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J14" s="43"/>
     </row>
-    <row r="15" spans="2:11" ht="16" thickBot="1">
+    <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="38"/>
       <c r="C15" s="34" t="s">
         <v>39</v>
@@ -3539,7 +3474,7 @@
       <c r="J15" s="97"/>
       <c r="K15" s="33"/>
     </row>
-    <row r="16" spans="2:11" ht="20" customHeight="1" thickBot="1">
+    <row r="16" spans="2:11" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -3556,43 +3491,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!update_attributes">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>165100</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>3949700</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3607,30 +3505,29 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="65" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="65" customWidth="1"/>
-    <col min="3" max="3" width="35.875" style="65" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="65" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="65" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="65" customWidth="1"/>
-    <col min="7" max="7" width="10.75" style="65" customWidth="1"/>
-    <col min="8" max="8" width="4.75" style="65" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="66" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="65" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="65" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="65" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="65" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="65" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="66" customWidth="1"/>
     <col min="10" max="10" width="3" style="66" customWidth="1"/>
-    <col min="11" max="11" width="8.75" style="66" customWidth="1"/>
-    <col min="12" max="12" width="3.25" style="66" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="66" customWidth="1"/>
-    <col min="14" max="14" width="2.75" style="66" customWidth="1"/>
-    <col min="15" max="16" width="8.5" style="66" customWidth="1"/>
-    <col min="17" max="17" width="2.75" style="66" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="66" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" style="66" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="66" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="66" customWidth="1"/>
+    <col min="15" max="16" width="8.42578125" style="66" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="66" customWidth="1"/>
     <col min="18" max="18" width="60" style="65" customWidth="1"/>
-    <col min="19" max="16384" width="10.625" style="65"/>
+    <col min="19" max="16384" width="10.7109375" style="65"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="16" thickBot="1"/>
-    <row r="2" spans="2:18">
+    <row r="1" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="67"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -3649,7 +3546,7 @@
       <c r="Q2" s="69"/>
       <c r="R2" s="70"/>
     </row>
-    <row r="3" spans="2:18" s="24" customFormat="1">
+    <row r="3" spans="2:18" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="23"/>
       <c r="C3" s="101" t="s">
         <v>29</v>
@@ -3679,14 +3576,14 @@
         <v>49</v>
       </c>
       <c r="P3" s="63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="63"/>
       <c r="R3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:18">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="71"/>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
@@ -3705,7 +3602,7 @@
       <c r="Q4" s="100"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="2:18" ht="16" thickBot="1">
+    <row r="5" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="71"/>
       <c r="C5" s="18" t="s">
         <v>47</v>
@@ -3726,7 +3623,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="2:18" ht="16" thickBot="1">
+    <row r="6" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="71"/>
       <c r="C6" s="107" t="s">
         <v>36</v>
@@ -3755,7 +3652,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
+    <row r="7" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="108" t="s">
         <v>37</v>
@@ -3788,7 +3685,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="112"/>
     </row>
-    <row r="8" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
+    <row r="8" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="108" t="s">
         <v>93</v>
@@ -3821,7 +3718,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
+    <row r="9" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="109" t="s">
         <v>38</v>
@@ -3850,10 +3747,10 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="2:18" s="6" customFormat="1" ht="16" thickBot="1">
+    <row r="10" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="130" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="109"/>
       <c r="E10" s="109"/>
@@ -3879,7 +3776,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="2:18" ht="16" thickBot="1">
+    <row r="11" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="71"/>
       <c r="C11" s="109" t="s">
         <v>39</v>
@@ -3912,7 +3809,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="112"/>
     </row>
-    <row r="12" spans="2:18" ht="16" thickBot="1">
+    <row r="12" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="76"/>
       <c r="C12" s="77"/>
       <c r="D12" s="77"/>
@@ -3931,37 +3828,32 @@
       <c r="Q12" s="77"/>
       <c r="R12" s="78"/>
     </row>
-    <row r="13" spans="2:18">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="2:18">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="2:18">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="2:18">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="15:18">
+    <row r="17" spans="15:18" x14ac:dyDescent="0.2">
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="15:18">
+    <row r="18" spans="15:18" x14ac:dyDescent="0.2">
       <c r="R18" s="112"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3976,23 +3868,23 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="45" customWidth="1"/>
-    <col min="2" max="2" width="3.375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="28.75" style="45" customWidth="1"/>
-    <col min="4" max="4" width="3.125" style="45" customWidth="1"/>
-    <col min="5" max="5" width="16.125" style="45" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="45" customWidth="1"/>
     <col min="6" max="6" width="5" style="45" customWidth="1"/>
-    <col min="7" max="7" width="10.25" style="45" customWidth="1"/>
-    <col min="8" max="10" width="12.125" style="45" customWidth="1"/>
-    <col min="11" max="11" width="33.125" style="46" customWidth="1"/>
-    <col min="12" max="12" width="87.25" style="45" customWidth="1"/>
-    <col min="13" max="16384" width="33.125" style="45"/>
+    <col min="7" max="7" width="10.28515625" style="45" customWidth="1"/>
+    <col min="8" max="10" width="12.140625" style="45" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="46" customWidth="1"/>
+    <col min="12" max="12" width="87.28515625" style="45" customWidth="1"/>
+    <col min="13" max="16384" width="33.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16" thickBot="1"/>
-    <row r="2" spans="2:12">
+    <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="47"/>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
@@ -4005,7 +3897,7 @@
       <c r="K2" s="49"/>
       <c r="L2" s="48"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="50"/>
       <c r="C3" s="51" t="s">
         <v>10</v>
@@ -4020,7 +3912,7 @@
       <c r="K3" s="52"/>
       <c r="L3" s="53"/>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="50"/>
       <c r="C4" s="53"/>
       <c r="D4" s="53"/>
@@ -4033,7 +3925,7 @@
       <c r="K4" s="54"/>
       <c r="L4" s="53"/>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="55"/>
       <c r="C5" s="56" t="s">
         <v>12</v>
@@ -4062,7 +3954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="50"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
@@ -4075,7 +3967,7 @@
       <c r="K6" s="52"/>
       <c r="L6" s="51"/>
     </row>
-    <row r="7" spans="2:12" ht="16">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="50"/>
       <c r="C7" s="116" t="s">
         <v>93</v>
@@ -4098,13 +3990,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="50"/>
       <c r="C8" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F8" s="115"/>
       <c r="G8" s="45" t="s">
@@ -4113,14 +4005,14 @@
       <c r="H8" s="45">
         <v>2006</v>
       </c>
-      <c r="K8" s="173" t="s">
+      <c r="K8" s="162" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="154" t="s">
         <v>101</v>
       </c>
-      <c r="L8" s="154" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="50"/>
       <c r="C9" s="58"/>
       <c r="D9" s="59"/>
@@ -4133,7 +4025,7 @@
       <c r="K9" s="54"/>
       <c r="L9" s="64"/>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="50"/>
       <c r="C10" s="157" t="s">
         <v>39</v>
@@ -4148,7 +4040,7 @@
       <c r="K10" s="54"/>
       <c r="L10" s="64"/>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="50"/>
       <c r="C11" s="117"/>
       <c r="D11" s="59"/>
@@ -4161,7 +4053,7 @@
       <c r="K11" s="54"/>
       <c r="L11" s="64"/>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="50"/>
       <c r="C12" s="58"/>
       <c r="D12" s="62"/>
@@ -4174,7 +4066,7 @@
       <c r="K12" s="61"/>
       <c r="L12" s="58"/>
     </row>
-    <row r="13" spans="2:12" ht="16">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="50"/>
       <c r="C13" s="116" t="s">
         <v>37</v>
@@ -4201,19 +4093,19 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="50"/>
       <c r="C15" s="62"/>
       <c r="E15" s="115"/>
       <c r="F15" s="115"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="50"/>
       <c r="C16" s="103"/>
       <c r="E16" s="115"/>
       <c r="F16" s="115"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="50"/>
       <c r="E17" s="115"/>
       <c r="F17" s="115"/>
@@ -4226,11 +4118,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4243,22 +4130,22 @@
       <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.625" style="132" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="132" customWidth="1"/>
     <col min="2" max="2" width="5" style="132" customWidth="1"/>
     <col min="3" max="3" width="7" style="132"/>
-    <col min="4" max="4" width="7.125" style="132" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="132" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="132"/>
     <col min="6" max="6" width="11" style="132" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.875" style="132" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="132" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.25" style="132" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="132" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="132" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="132" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="7" style="132"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:45" ht="17" thickBot="1"/>
-    <row r="2" spans="2:45" s="135" customFormat="1">
+    <row r="1" spans="2:45" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:45" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="133"/>
       <c r="C2" s="134" t="s">
         <v>24</v>
@@ -4286,7 +4173,7 @@
       <c r="T2" s="134"/>
       <c r="U2" s="134"/>
     </row>
-    <row r="3" spans="2:45">
+    <row r="3" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B3" s="136"/>
       <c r="C3" s="137"/>
       <c r="D3" s="137"/>
@@ -4308,7 +4195,7 @@
       <c r="T3" s="137"/>
       <c r="U3" s="137"/>
     </row>
-    <row r="4" spans="2:45" s="139" customFormat="1">
+    <row r="4" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="136"/>
       <c r="C4" s="138" t="s">
         <v>63</v>
@@ -4356,7 +4243,7 @@
       <c r="AR4" s="144"/>
       <c r="AS4" s="144"/>
     </row>
-    <row r="5" spans="2:45" s="139" customFormat="1">
+    <row r="5" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="136"/>
       <c r="C5" s="138"/>
       <c r="D5" s="144"/>
@@ -4402,12 +4289,12 @@
       <c r="AR5" s="144"/>
       <c r="AS5" s="144"/>
     </row>
-    <row r="6" spans="2:45" s="139" customFormat="1" ht="18">
+    <row r="6" spans="2:45" s="139" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="B6" s="136"/>
       <c r="C6" s="144"/>
       <c r="D6" s="144"/>
       <c r="F6" s="145" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" s="144"/>
       <c r="H6" s="144"/>
@@ -4449,7 +4336,7 @@
       <c r="AR6" s="144"/>
       <c r="AS6" s="144"/>
     </row>
-    <row r="7" spans="2:45" s="139" customFormat="1">
+    <row r="7" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="136"/>
       <c r="C7" s="144"/>
       <c r="D7" s="144"/>
@@ -4498,7 +4385,7 @@
       <c r="AR7" s="144"/>
       <c r="AS7" s="144"/>
     </row>
-    <row r="8" spans="2:45" s="139" customFormat="1">
+    <row r="8" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="136"/>
       <c r="C8" s="144"/>
       <c r="D8" s="144"/>
@@ -4549,7 +4436,7 @@
       <c r="AR8" s="144"/>
       <c r="AS8" s="144"/>
     </row>
-    <row r="9" spans="2:45" s="139" customFormat="1">
+    <row r="9" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="136"/>
       <c r="C9" s="144"/>
       <c r="D9" s="144"/>
@@ -4600,7 +4487,7 @@
       <c r="AR9" s="144"/>
       <c r="AS9" s="144"/>
     </row>
-    <row r="10" spans="2:45" s="139" customFormat="1">
+    <row r="10" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="136"/>
       <c r="C10" s="144"/>
       <c r="D10" s="144"/>
@@ -4646,7 +4533,7 @@
       <c r="AR10" s="144"/>
       <c r="AS10" s="144"/>
     </row>
-    <row r="11" spans="2:45" s="139" customFormat="1">
+    <row r="11" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="136"/>
       <c r="C11" s="144"/>
       <c r="D11" s="144"/>
@@ -4692,7 +4579,7 @@
       <c r="AR11" s="144"/>
       <c r="AS11" s="144"/>
     </row>
-    <row r="12" spans="2:45" s="139" customFormat="1">
+    <row r="12" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="136"/>
       <c r="C12" s="144"/>
       <c r="D12" s="144"/>
@@ -4738,7 +4625,7 @@
       <c r="AR12" s="144"/>
       <c r="AS12" s="144"/>
     </row>
-    <row r="13" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="13" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="136"/>
       <c r="C13" s="144"/>
       <c r="D13" s="144"/>
@@ -4784,7 +4671,7 @@
       <c r="AR13" s="144"/>
       <c r="AS13" s="144"/>
     </row>
-    <row r="14" spans="2:45" s="135" customFormat="1">
+    <row r="14" spans="2:45" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="134"/>
       <c r="C14" s="134" t="s">
         <v>24</v>
@@ -4812,7 +4699,7 @@
       <c r="T14" s="134"/>
       <c r="U14" s="134"/>
     </row>
-    <row r="15" spans="2:45" s="139" customFormat="1">
+    <row r="15" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="136"/>
       <c r="C15" s="144"/>
       <c r="D15" s="144"/>
@@ -4838,7 +4725,7 @@
       <c r="X15" s="144"/>
       <c r="Y15" s="144"/>
     </row>
-    <row r="16" spans="2:45" s="139" customFormat="1">
+    <row r="16" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="136"/>
       <c r="C16" s="144" t="s">
         <v>68</v>
@@ -4886,7 +4773,7 @@
       <c r="AR16" s="144"/>
       <c r="AS16" s="144"/>
     </row>
-    <row r="17" spans="2:45" s="139" customFormat="1">
+    <row r="17" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="136"/>
       <c r="C17" s="138" t="s">
         <v>69</v>
@@ -4934,7 +4821,7 @@
       <c r="AR17" s="144"/>
       <c r="AS17" s="144"/>
     </row>
-    <row r="18" spans="2:45" s="139" customFormat="1">
+    <row r="18" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="136"/>
       <c r="C18" s="144"/>
       <c r="D18" s="144"/>
@@ -4980,7 +4867,7 @@
       <c r="AR18" s="144"/>
       <c r="AS18" s="144"/>
     </row>
-    <row r="19" spans="2:45" s="139" customFormat="1">
+    <row r="19" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="136"/>
       <c r="C19" s="144"/>
       <c r="D19" s="144"/>
@@ -5026,7 +4913,7 @@
       <c r="AR19" s="144"/>
       <c r="AS19" s="144"/>
     </row>
-    <row r="20" spans="2:45" s="139" customFormat="1">
+    <row r="20" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="136"/>
       <c r="C20" s="144"/>
       <c r="D20" s="144"/>
@@ -5072,7 +4959,7 @@
       <c r="AR20" s="144"/>
       <c r="AS20" s="144"/>
     </row>
-    <row r="21" spans="2:45" s="139" customFormat="1">
+    <row r="21" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="136"/>
       <c r="C21" s="144"/>
       <c r="D21" s="144"/>
@@ -5118,7 +5005,7 @@
       <c r="AR21" s="144"/>
       <c r="AS21" s="144"/>
     </row>
-    <row r="22" spans="2:45" s="139" customFormat="1">
+    <row r="22" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="136"/>
       <c r="C22" s="144"/>
       <c r="D22" s="144"/>
@@ -5164,7 +5051,7 @@
       <c r="AR22" s="144"/>
       <c r="AS22" s="144"/>
     </row>
-    <row r="23" spans="2:45" s="139" customFormat="1">
+    <row r="23" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="136"/>
       <c r="C23" s="144"/>
       <c r="D23" s="144"/>
@@ -5210,7 +5097,7 @@
       <c r="AR23" s="144"/>
       <c r="AS23" s="144"/>
     </row>
-    <row r="24" spans="2:45" s="139" customFormat="1">
+    <row r="24" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="136"/>
       <c r="C24" s="144"/>
       <c r="D24" s="144"/>
@@ -5256,7 +5143,7 @@
       <c r="AR24" s="144"/>
       <c r="AS24" s="144"/>
     </row>
-    <row r="25" spans="2:45" s="139" customFormat="1">
+    <row r="25" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="136"/>
       <c r="C25" s="144"/>
       <c r="D25" s="144"/>
@@ -5302,7 +5189,7 @@
       <c r="AR25" s="144"/>
       <c r="AS25" s="144"/>
     </row>
-    <row r="26" spans="2:45" s="139" customFormat="1">
+    <row r="26" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="136"/>
       <c r="C26" s="144"/>
       <c r="D26" s="144"/>
@@ -5348,7 +5235,7 @@
       <c r="AR26" s="144"/>
       <c r="AS26" s="144"/>
     </row>
-    <row r="27" spans="2:45" s="139" customFormat="1">
+    <row r="27" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="136"/>
       <c r="C27" s="144"/>
       <c r="D27" s="144"/>
@@ -5394,7 +5281,7 @@
       <c r="AR27" s="144"/>
       <c r="AS27" s="144"/>
     </row>
-    <row r="28" spans="2:45" s="139" customFormat="1">
+    <row r="28" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="136"/>
       <c r="C28" s="144"/>
       <c r="D28" s="144"/>
@@ -5440,7 +5327,7 @@
       <c r="AR28" s="144"/>
       <c r="AS28" s="144"/>
     </row>
-    <row r="29" spans="2:45" s="139" customFormat="1">
+    <row r="29" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="136"/>
       <c r="C29" s="144"/>
       <c r="D29" s="144"/>
@@ -5486,7 +5373,7 @@
       <c r="AR29" s="144"/>
       <c r="AS29" s="144"/>
     </row>
-    <row r="30" spans="2:45" s="139" customFormat="1">
+    <row r="30" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="136"/>
       <c r="C30" s="144"/>
       <c r="D30" s="144"/>
@@ -5532,7 +5419,7 @@
       <c r="AR30" s="144"/>
       <c r="AS30" s="144"/>
     </row>
-    <row r="31" spans="2:45" s="139" customFormat="1">
+    <row r="31" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="136"/>
       <c r="C31" s="144"/>
       <c r="D31" s="144"/>
@@ -5578,7 +5465,7 @@
       <c r="AR31" s="144"/>
       <c r="AS31" s="144"/>
     </row>
-    <row r="32" spans="2:45" s="139" customFormat="1">
+    <row r="32" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="136"/>
       <c r="C32" s="144"/>
       <c r="D32" s="144"/>
@@ -5624,7 +5511,7 @@
       <c r="AR32" s="144"/>
       <c r="AS32" s="144"/>
     </row>
-    <row r="33" spans="2:45" s="139" customFormat="1">
+    <row r="33" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="136"/>
       <c r="C33" s="144"/>
       <c r="D33" s="144"/>
@@ -5670,7 +5557,7 @@
       <c r="AR33" s="144"/>
       <c r="AS33" s="144"/>
     </row>
-    <row r="34" spans="2:45" s="139" customFormat="1">
+    <row r="34" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="136"/>
       <c r="C34" s="144"/>
       <c r="D34" s="144"/>
@@ -5716,7 +5603,7 @@
       <c r="AR34" s="144"/>
       <c r="AS34" s="144"/>
     </row>
-    <row r="35" spans="2:45" s="139" customFormat="1">
+    <row r="35" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="136"/>
       <c r="C35" s="144"/>
       <c r="D35" s="144"/>
@@ -5762,7 +5649,7 @@
       <c r="AR35" s="144"/>
       <c r="AS35" s="144"/>
     </row>
-    <row r="36" spans="2:45" s="139" customFormat="1">
+    <row r="36" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="136"/>
       <c r="C36" s="144"/>
       <c r="D36" s="144"/>
@@ -5808,7 +5695,7 @@
       <c r="AR36" s="144"/>
       <c r="AS36" s="144"/>
     </row>
-    <row r="37" spans="2:45" s="139" customFormat="1">
+    <row r="37" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="136"/>
       <c r="C37" s="144"/>
       <c r="D37" s="144">
@@ -5856,7 +5743,7 @@
       <c r="AR37" s="144"/>
       <c r="AS37" s="144"/>
     </row>
-    <row r="38" spans="2:45" s="139" customFormat="1">
+    <row r="38" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="136"/>
       <c r="C38" s="144"/>
       <c r="D38" s="144"/>
@@ -5908,7 +5795,7 @@
       <c r="AR38" s="144"/>
       <c r="AS38" s="144"/>
     </row>
-    <row r="39" spans="2:45" s="139" customFormat="1">
+    <row r="39" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="136"/>
       <c r="C39" s="144"/>
       <c r="D39" s="144"/>
@@ -5961,7 +5848,7 @@
       <c r="AR39" s="144"/>
       <c r="AS39" s="144"/>
     </row>
-    <row r="40" spans="2:45" s="139" customFormat="1">
+    <row r="40" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="136"/>
       <c r="C40" s="144"/>
       <c r="D40" s="144"/>
@@ -6013,7 +5900,7 @@
       <c r="AR40" s="144"/>
       <c r="AS40" s="144"/>
     </row>
-    <row r="41" spans="2:45" s="139" customFormat="1">
+    <row r="41" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="136"/>
       <c r="C41" s="144"/>
       <c r="D41" s="144"/>
@@ -6066,7 +5953,7 @@
       <c r="AR41" s="144"/>
       <c r="AS41" s="144"/>
     </row>
-    <row r="42" spans="2:45" s="139" customFormat="1">
+    <row r="42" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="136"/>
       <c r="C42" s="144"/>
       <c r="D42" s="144"/>
@@ -6117,7 +6004,7 @@
       <c r="AR42" s="144"/>
       <c r="AS42" s="144"/>
     </row>
-    <row r="43" spans="2:45" s="139" customFormat="1">
+    <row r="43" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="136"/>
       <c r="C43" s="144"/>
       <c r="D43" s="144"/>
@@ -6168,7 +6055,7 @@
       <c r="AR43" s="144"/>
       <c r="AS43" s="144"/>
     </row>
-    <row r="44" spans="2:45" s="139" customFormat="1">
+    <row r="44" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="136"/>
       <c r="C44" s="144"/>
       <c r="D44" s="144"/>
@@ -6214,7 +6101,7 @@
       <c r="AR44" s="144"/>
       <c r="AS44" s="144"/>
     </row>
-    <row r="45" spans="2:45" s="139" customFormat="1">
+    <row r="45" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="136"/>
       <c r="C45" s="144"/>
       <c r="D45" s="144"/>
@@ -6264,7 +6151,7 @@
       <c r="AR45" s="144"/>
       <c r="AS45" s="144"/>
     </row>
-    <row r="46" spans="2:45" s="139" customFormat="1">
+    <row r="46" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="136"/>
       <c r="C46" s="144"/>
       <c r="D46" s="144"/>
@@ -6310,7 +6197,7 @@
       <c r="AR46" s="144"/>
       <c r="AS46" s="144"/>
     </row>
-    <row r="47" spans="2:45" s="139" customFormat="1">
+    <row r="47" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="136"/>
       <c r="C47" s="144"/>
       <c r="D47" s="144"/>
@@ -6356,7 +6243,7 @@
       <c r="AR47" s="144"/>
       <c r="AS47" s="144"/>
     </row>
-    <row r="48" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="48" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="136"/>
       <c r="C48" s="144"/>
       <c r="D48" s="144"/>
@@ -6402,7 +6289,7 @@
       <c r="AR48" s="144"/>
       <c r="AS48" s="144"/>
     </row>
-    <row r="49" spans="2:45" s="135" customFormat="1">
+    <row r="49" spans="2:45" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B49" s="134"/>
       <c r="C49" s="134" t="s">
         <v>24</v>
@@ -6430,7 +6317,7 @@
       <c r="T49" s="134"/>
       <c r="U49" s="134"/>
     </row>
-    <row r="50" spans="2:45" s="139" customFormat="1">
+    <row r="50" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="136"/>
       <c r="C50" s="144"/>
       <c r="D50" s="144"/>
@@ -6456,7 +6343,7 @@
       <c r="X50" s="144"/>
       <c r="Y50" s="144"/>
     </row>
-    <row r="51" spans="2:45" s="139" customFormat="1">
+    <row r="51" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="136"/>
       <c r="C51" s="138" t="s">
         <v>79</v>
@@ -6504,17 +6391,17 @@
       <c r="AR51" s="144"/>
       <c r="AS51" s="144"/>
     </row>
-    <row r="52" spans="2:45" s="139" customFormat="1">
+    <row r="52" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="136"/>
       <c r="C52" s="144"/>
       <c r="D52" s="144"/>
       <c r="E52" s="144"/>
       <c r="F52" s="144"/>
-      <c r="G52" s="171" t="s">
+      <c r="G52" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="H52" s="172"/>
-      <c r="I52" s="172"/>
+      <c r="H52" s="173"/>
+      <c r="I52" s="173"/>
       <c r="J52" s="144"/>
       <c r="K52" s="144"/>
       <c r="L52" s="144"/>
@@ -6552,7 +6439,7 @@
       <c r="AR52" s="144"/>
       <c r="AS52" s="144"/>
     </row>
-    <row r="53" spans="2:45" s="139" customFormat="1">
+    <row r="53" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="136"/>
       <c r="C53" s="144"/>
       <c r="D53" s="144"/>
@@ -6604,7 +6491,7 @@
       <c r="AR53" s="144"/>
       <c r="AS53" s="144"/>
     </row>
-    <row r="54" spans="2:45" s="139" customFormat="1">
+    <row r="54" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="136"/>
       <c r="C54" s="144"/>
       <c r="D54" s="144"/>
@@ -6656,7 +6543,7 @@
       <c r="AR54" s="144"/>
       <c r="AS54" s="144"/>
     </row>
-    <row r="55" spans="2:45" s="139" customFormat="1">
+    <row r="55" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="136"/>
       <c r="C55" s="144"/>
       <c r="D55" s="144"/>
@@ -6708,7 +6595,7 @@
       <c r="AR55" s="144"/>
       <c r="AS55" s="144"/>
     </row>
-    <row r="56" spans="2:45" s="139" customFormat="1">
+    <row r="56" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="136"/>
       <c r="C56" s="144"/>
       <c r="D56" s="144"/>
@@ -6760,7 +6647,7 @@
       <c r="AR56" s="144"/>
       <c r="AS56" s="144"/>
     </row>
-    <row r="57" spans="2:45" s="139" customFormat="1">
+    <row r="57" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="136"/>
       <c r="C57" s="144"/>
       <c r="D57" s="144"/>
@@ -6812,7 +6699,7 @@
       <c r="AR57" s="144"/>
       <c r="AS57" s="144"/>
     </row>
-    <row r="58" spans="2:45" s="139" customFormat="1">
+    <row r="58" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="136"/>
       <c r="C58" s="144"/>
       <c r="D58" s="144"/>
@@ -6864,7 +6751,7 @@
       <c r="AR58" s="144"/>
       <c r="AS58" s="144"/>
     </row>
-    <row r="59" spans="2:45" s="139" customFormat="1">
+    <row r="59" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="136"/>
       <c r="C59" s="144"/>
       <c r="D59" s="144"/>
@@ -6916,7 +6803,7 @@
       <c r="AR59" s="144"/>
       <c r="AS59" s="144"/>
     </row>
-    <row r="60" spans="2:45" s="139" customFormat="1">
+    <row r="60" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="136"/>
       <c r="C60" s="144"/>
       <c r="D60" s="144"/>
@@ -6968,7 +6855,7 @@
       <c r="AR60" s="144"/>
       <c r="AS60" s="144"/>
     </row>
-    <row r="61" spans="2:45" s="139" customFormat="1">
+    <row r="61" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="136"/>
       <c r="C61" s="144"/>
       <c r="D61" s="144"/>
@@ -7020,7 +6907,7 @@
       <c r="AR61" s="144"/>
       <c r="AS61" s="144"/>
     </row>
-    <row r="62" spans="2:45" s="139" customFormat="1">
+    <row r="62" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="136"/>
       <c r="C62" s="144"/>
       <c r="D62" s="144"/>
@@ -7072,7 +6959,7 @@
       <c r="AR62" s="144"/>
       <c r="AS62" s="144"/>
     </row>
-    <row r="63" spans="2:45" s="139" customFormat="1">
+    <row r="63" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="136"/>
       <c r="C63" s="144"/>
       <c r="D63" s="144"/>
@@ -7124,7 +7011,7 @@
       <c r="AR63" s="144"/>
       <c r="AS63" s="144"/>
     </row>
-    <row r="64" spans="2:45" s="139" customFormat="1">
+    <row r="64" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="136"/>
       <c r="C64" s="144"/>
       <c r="D64" s="144"/>
@@ -7176,7 +7063,7 @@
       <c r="AR64" s="144"/>
       <c r="AS64" s="144"/>
     </row>
-    <row r="65" spans="2:45" s="139" customFormat="1">
+    <row r="65" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="136"/>
       <c r="C65" s="144"/>
       <c r="D65" s="144"/>
@@ -7228,7 +7115,7 @@
       <c r="AR65" s="144"/>
       <c r="AS65" s="144"/>
     </row>
-    <row r="66" spans="2:45" s="139" customFormat="1">
+    <row r="66" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="136"/>
       <c r="C66" s="144"/>
       <c r="D66" s="144"/>
@@ -7273,7 +7160,7 @@
       <c r="AR66" s="144"/>
       <c r="AS66" s="144"/>
     </row>
-    <row r="67" spans="2:45" s="139" customFormat="1">
+    <row r="67" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="136"/>
       <c r="C67" s="144"/>
       <c r="D67" s="144"/>
@@ -7319,7 +7206,7 @@
       <c r="AR67" s="144"/>
       <c r="AS67" s="144"/>
     </row>
-    <row r="68" spans="2:45" s="139" customFormat="1">
+    <row r="68" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="136"/>
       <c r="C68" s="144"/>
       <c r="D68" s="144"/>
@@ -7370,7 +7257,7 @@
       <c r="AR68" s="144"/>
       <c r="AS68" s="144"/>
     </row>
-    <row r="69" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="69" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="136"/>
       <c r="C69" s="144"/>
       <c r="D69" s="144"/>
@@ -7420,7 +7307,7 @@
       <c r="AR69" s="144"/>
       <c r="AS69" s="144"/>
     </row>
-    <row r="70" spans="2:45" s="135" customFormat="1">
+    <row r="70" spans="2:45" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="134"/>
       <c r="C70" s="134" t="s">
         <v>24</v>
@@ -7448,10 +7335,10 @@
       <c r="T70" s="134"/>
       <c r="U70" s="134"/>
     </row>
-    <row r="71" spans="2:45" s="139" customFormat="1">
+    <row r="71" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="136"/>
       <c r="C71" s="152" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D71" s="144"/>
       <c r="E71" s="144"/>
@@ -7476,7 +7363,7 @@
       <c r="X71" s="144"/>
       <c r="Y71" s="144"/>
     </row>
-    <row r="72" spans="2:45" s="139" customFormat="1">
+    <row r="72" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="136"/>
       <c r="C72" s="144"/>
       <c r="D72" s="144"/>
@@ -7502,7 +7389,7 @@
       <c r="X72" s="144"/>
       <c r="Y72" s="144"/>
     </row>
-    <row r="73" spans="2:45" s="139" customFormat="1">
+    <row r="73" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="136"/>
       <c r="C73" s="144"/>
       <c r="D73" s="144"/>
@@ -7528,7 +7415,7 @@
       <c r="X73" s="144"/>
       <c r="Y73" s="144"/>
     </row>
-    <row r="74" spans="2:45" s="139" customFormat="1">
+    <row r="74" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="136"/>
       <c r="C74" s="144"/>
       <c r="D74" s="144">
@@ -7537,7 +7424,7 @@
       <c r="E74" s="144"/>
       <c r="F74" s="144"/>
       <c r="G74" s="158" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H74" s="144"/>
       <c r="I74" s="144"/>
@@ -7558,7 +7445,7 @@
       <c r="X74" s="144"/>
       <c r="Y74" s="144"/>
     </row>
-    <row r="75" spans="2:45" s="139" customFormat="1">
+    <row r="75" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="136"/>
       <c r="C75" s="144"/>
       <c r="D75" s="139">
@@ -7567,7 +7454,7 @@
       <c r="E75" s="144"/>
       <c r="F75" s="144"/>
       <c r="G75" s="144" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H75" s="144"/>
       <c r="I75" s="144"/>
@@ -7588,7 +7475,7 @@
       <c r="X75" s="144"/>
       <c r="Y75" s="144"/>
     </row>
-    <row r="76" spans="2:45" s="139" customFormat="1">
+    <row r="76" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="136"/>
       <c r="C76" s="144"/>
       <c r="J76" s="144"/>
@@ -7608,7 +7495,7 @@
       <c r="X76" s="144"/>
       <c r="Y76" s="144"/>
     </row>
-    <row r="77" spans="2:45" s="139" customFormat="1">
+    <row r="77" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="136"/>
       <c r="C77" s="144"/>
       <c r="G77" s="148">
@@ -7616,10 +7503,10 @@
         <v>7.3300000000000004E-2</v>
       </c>
       <c r="H77" s="148" t="s">
+        <v>108</v>
+      </c>
+      <c r="I77" s="148" t="s">
         <v>109</v>
-      </c>
-      <c r="I77" s="148" t="s">
-        <v>110</v>
       </c>
       <c r="J77" s="144"/>
       <c r="K77" s="144"/>
@@ -7638,7 +7525,7 @@
       <c r="X77" s="144"/>
       <c r="Y77" s="144"/>
     </row>
-    <row r="78" spans="2:45" s="139" customFormat="1">
+    <row r="78" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="136"/>
       <c r="C78" s="144"/>
       <c r="G78" s="148">
@@ -7646,7 +7533,7 @@
         <v>7.0800000000000002E-2</v>
       </c>
       <c r="H78" s="148" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I78" s="148"/>
       <c r="J78" s="144"/>
@@ -7666,7 +7553,7 @@
       <c r="X78" s="144"/>
       <c r="Y78" s="144"/>
     </row>
-    <row r="79" spans="2:45" s="139" customFormat="1">
+    <row r="79" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="136"/>
       <c r="C79" s="144"/>
       <c r="G79" s="148">
@@ -7674,7 +7561,7 @@
         <v>7.9600000000000004E-2</v>
       </c>
       <c r="H79" s="148" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I79" s="148"/>
       <c r="J79" s="144"/>
@@ -7694,7 +7581,7 @@
       <c r="X79" s="144"/>
       <c r="Y79" s="144"/>
     </row>
-    <row r="80" spans="2:45" s="139" customFormat="1">
+    <row r="80" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="136"/>
       <c r="C80" s="144"/>
       <c r="D80" s="144"/>
@@ -7705,7 +7592,7 @@
         <v>7.456666666666667E-2</v>
       </c>
       <c r="H80" s="144" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I80" s="144"/>
       <c r="J80" s="144"/>
@@ -7725,7 +7612,7 @@
       <c r="X80" s="144"/>
       <c r="Y80" s="144"/>
     </row>
-    <row r="81" spans="2:25" s="139" customFormat="1">
+    <row r="81" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="136"/>
       <c r="C81" s="144"/>
       <c r="J81" s="144"/>
@@ -7745,7 +7632,7 @@
       <c r="X81" s="144"/>
       <c r="Y81" s="144"/>
     </row>
-    <row r="82" spans="2:25" s="139" customFormat="1">
+    <row r="82" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="136"/>
       <c r="C82" s="144"/>
       <c r="J82" s="144"/>
@@ -7765,7 +7652,7 @@
       <c r="X82" s="144"/>
       <c r="Y82" s="144"/>
     </row>
-    <row r="83" spans="2:25" s="139" customFormat="1">
+    <row r="83" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="136"/>
       <c r="C83" s="144"/>
       <c r="J83" s="144"/>
@@ -7785,7 +7672,7 @@
       <c r="X83" s="144"/>
       <c r="Y83" s="144"/>
     </row>
-    <row r="84" spans="2:25" s="139" customFormat="1">
+    <row r="84" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B84" s="136"/>
       <c r="C84" s="144"/>
       <c r="D84" s="144"/>
@@ -7811,7 +7698,7 @@
       <c r="X84" s="144"/>
       <c r="Y84" s="144"/>
     </row>
-    <row r="85" spans="2:25" s="139" customFormat="1">
+    <row r="85" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="136"/>
       <c r="C85" s="144"/>
       <c r="D85" s="144"/>
@@ -7837,7 +7724,7 @@
       <c r="X85" s="144"/>
       <c r="Y85" s="144"/>
     </row>
-    <row r="86" spans="2:25" s="139" customFormat="1">
+    <row r="86" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B86" s="136"/>
       <c r="C86" s="144"/>
       <c r="D86" s="144"/>
@@ -7859,7 +7746,7 @@
       <c r="X86" s="144"/>
       <c r="Y86" s="144"/>
     </row>
-    <row r="87" spans="2:25" s="139" customFormat="1">
+    <row r="87" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B87" s="136"/>
       <c r="C87" s="144"/>
       <c r="D87" s="144"/>
@@ -7881,7 +7768,7 @@
       <c r="X87" s="144"/>
       <c r="Y87" s="144"/>
     </row>
-    <row r="88" spans="2:25" s="139" customFormat="1">
+    <row r="88" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="136"/>
       <c r="C88" s="144"/>
       <c r="D88" s="144"/>
@@ -7903,7 +7790,7 @@
       <c r="X88" s="144"/>
       <c r="Y88" s="144"/>
     </row>
-    <row r="89" spans="2:25" s="139" customFormat="1">
+    <row r="89" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B89" s="136"/>
       <c r="C89" s="144"/>
       <c r="D89" s="144"/>
@@ -7929,7 +7816,7 @@
       <c r="X89" s="144"/>
       <c r="Y89" s="144"/>
     </row>
-    <row r="90" spans="2:25" s="139" customFormat="1">
+    <row r="90" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B90" s="136"/>
       <c r="C90" s="144"/>
       <c r="D90" s="144"/>
@@ -7952,7 +7839,7 @@
       <c r="X90" s="144"/>
       <c r="Y90" s="144"/>
     </row>
-    <row r="91" spans="2:25" s="139" customFormat="1">
+    <row r="91" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B91" s="136"/>
       <c r="C91" s="144"/>
       <c r="D91" s="144"/>
@@ -7975,7 +7862,7 @@
       <c r="X91" s="144"/>
       <c r="Y91" s="144"/>
     </row>
-    <row r="92" spans="2:25" s="139" customFormat="1">
+    <row r="92" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B92" s="136"/>
       <c r="C92" s="144"/>
       <c r="D92" s="144"/>
@@ -7998,7 +7885,7 @@
       <c r="X92" s="144"/>
       <c r="Y92" s="144"/>
     </row>
-    <row r="93" spans="2:25" s="139" customFormat="1">
+    <row r="93" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B93" s="136"/>
       <c r="C93" s="144"/>
       <c r="D93" s="144"/>
@@ -8021,7 +7908,7 @@
       <c r="X93" s="144"/>
       <c r="Y93" s="144"/>
     </row>
-    <row r="94" spans="2:25" s="139" customFormat="1">
+    <row r="94" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B94" s="136"/>
       <c r="C94" s="144"/>
       <c r="D94" s="144"/>
@@ -8047,7 +7934,7 @@
       <c r="X94" s="144"/>
       <c r="Y94" s="144"/>
     </row>
-    <row r="95" spans="2:25" s="139" customFormat="1">
+    <row r="95" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B95" s="136"/>
       <c r="C95" s="144"/>
       <c r="D95" s="144"/>
@@ -8073,7 +7960,7 @@
       <c r="X95" s="144"/>
       <c r="Y95" s="144"/>
     </row>
-    <row r="96" spans="2:25" s="139" customFormat="1">
+    <row r="96" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="136"/>
       <c r="C96" s="144"/>
       <c r="D96" s="144"/>
@@ -8099,28 +7986,28 @@
       <c r="X96" s="144"/>
       <c r="Y96" s="144"/>
     </row>
-    <row r="97" spans="2:45" s="139" customFormat="1">
+    <row r="97" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B97" s="136"/>
     </row>
-    <row r="98" spans="2:45" s="139" customFormat="1">
+    <row r="98" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B98" s="136"/>
     </row>
-    <row r="99" spans="2:45" s="139" customFormat="1">
+    <row r="99" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B99" s="136"/>
     </row>
-    <row r="100" spans="2:45" s="139" customFormat="1">
+    <row r="100" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B100" s="136"/>
     </row>
-    <row r="101" spans="2:45" s="139" customFormat="1">
+    <row r="101" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B101" s="136"/>
     </row>
-    <row r="102" spans="2:45" s="139" customFormat="1">
+    <row r="102" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B102" s="136"/>
     </row>
-    <row r="103" spans="2:45" s="139" customFormat="1">
+    <row r="103" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B103" s="136"/>
     </row>
-    <row r="104" spans="2:45" s="139" customFormat="1">
+    <row r="104" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B104" s="136"/>
       <c r="D104" s="144">
         <v>1.24</v>
@@ -8130,13 +8017,13 @@
         <v>73300</v>
       </c>
       <c r="H104" s="144" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I104" s="144" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="105" spans="2:45" s="139" customFormat="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B105" s="136"/>
       <c r="D105" s="144"/>
       <c r="F105" s="144"/>
@@ -8145,11 +8032,11 @@
         <v>1000000</v>
       </c>
       <c r="H105" s="144" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I105" s="144"/>
     </row>
-    <row r="106" spans="2:45" s="139" customFormat="1">
+    <row r="106" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B106" s="136"/>
       <c r="D106" s="144"/>
       <c r="F106" s="159"/>
@@ -8158,11 +8045,11 @@
         <v>7.3300000000000004E-2</v>
       </c>
       <c r="H106" s="159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I106" s="144"/>
     </row>
-    <row r="107" spans="2:45" s="139" customFormat="1">
+    <row r="107" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B107" s="136"/>
       <c r="D107" s="144"/>
       <c r="F107" s="159"/>
@@ -8170,13 +8057,13 @@
       <c r="H107" s="160"/>
       <c r="I107" s="144"/>
     </row>
-    <row r="108" spans="2:45" s="139" customFormat="1">
+    <row r="108" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B108" s="136"/>
       <c r="F108" s="161"/>
       <c r="G108" s="161"/>
       <c r="H108" s="161"/>
     </row>
-    <row r="109" spans="2:45" s="139" customFormat="1">
+    <row r="109" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B109" s="137"/>
       <c r="C109" s="144"/>
       <c r="D109" s="144"/>
@@ -8221,7 +8108,7 @@
       <c r="AR109" s="144"/>
       <c r="AS109" s="144"/>
     </row>
-    <row r="110" spans="2:45" s="139" customFormat="1">
+    <row r="110" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B110" s="137"/>
       <c r="C110" s="144"/>
       <c r="D110" s="144"/>
@@ -8266,7 +8153,7 @@
       <c r="AR110" s="144"/>
       <c r="AS110" s="144"/>
     </row>
-    <row r="111" spans="2:45" s="139" customFormat="1">
+    <row r="111" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B111" s="137"/>
       <c r="C111" s="144"/>
       <c r="D111" s="144"/>
@@ -8311,7 +8198,7 @@
       <c r="AR111" s="144"/>
       <c r="AS111" s="144"/>
     </row>
-    <row r="112" spans="2:45" s="139" customFormat="1">
+    <row r="112" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B112" s="137"/>
       <c r="C112" s="144"/>
       <c r="D112" s="144"/>
@@ -8356,7 +8243,7 @@
       <c r="AR112" s="144"/>
       <c r="AS112" s="144"/>
     </row>
-    <row r="113" spans="2:45" s="139" customFormat="1">
+    <row r="113" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B113" s="137"/>
       <c r="C113" s="144"/>
       <c r="D113" s="144"/>
@@ -8401,7 +8288,7 @@
       <c r="AR113" s="144"/>
       <c r="AS113" s="144"/>
     </row>
-    <row r="114" spans="2:45" s="139" customFormat="1">
+    <row r="114" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B114" s="137"/>
       <c r="C114" s="144"/>
       <c r="D114" s="144"/>
@@ -8411,10 +8298,10 @@
         <v>70800</v>
       </c>
       <c r="H114" s="159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I114" s="148" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J114" s="144"/>
       <c r="K114" s="144"/>
@@ -8453,7 +8340,7 @@
       <c r="AR114" s="144"/>
       <c r="AS114" s="144"/>
     </row>
-    <row r="115" spans="2:45" s="139" customFormat="1">
+    <row r="115" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B115" s="137"/>
       <c r="C115" s="144"/>
       <c r="D115" s="144"/>
@@ -8464,7 +8351,7 @@
         <v>1000000</v>
       </c>
       <c r="H115" s="159" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I115" s="148"/>
       <c r="J115" s="144"/>
@@ -8504,7 +8391,7 @@
       <c r="AR115" s="144"/>
       <c r="AS115" s="144"/>
     </row>
-    <row r="116" spans="2:45" s="139" customFormat="1">
+    <row r="116" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B116" s="137"/>
       <c r="C116" s="144"/>
       <c r="D116" s="144"/>
@@ -8515,7 +8402,7 @@
         <v>7.0800000000000002E-2</v>
       </c>
       <c r="H116" s="159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I116" s="148"/>
       <c r="J116" s="144"/>
@@ -8555,7 +8442,7 @@
       <c r="AR116" s="144"/>
       <c r="AS116" s="144"/>
     </row>
-    <row r="117" spans="2:45" s="139" customFormat="1">
+    <row r="117" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B117" s="137"/>
       <c r="C117" s="144"/>
       <c r="D117" s="144"/>
@@ -8564,10 +8451,10 @@
         <v>79600</v>
       </c>
       <c r="H117" s="159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I117" s="148" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J117" s="144"/>
       <c r="K117" s="144"/>
@@ -8606,7 +8493,7 @@
       <c r="AR117" s="144"/>
       <c r="AS117" s="144"/>
     </row>
-    <row r="118" spans="2:45" s="139" customFormat="1">
+    <row r="118" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B118" s="137"/>
       <c r="C118" s="144"/>
       <c r="D118" s="144"/>
@@ -8616,7 +8503,7 @@
         <v>1000000</v>
       </c>
       <c r="H118" s="159" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I118" s="148"/>
       <c r="J118" s="144"/>
@@ -8656,7 +8543,7 @@
       <c r="AR118" s="144"/>
       <c r="AS118" s="144"/>
     </row>
-    <row r="119" spans="2:45" s="139" customFormat="1">
+    <row r="119" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B119" s="137"/>
       <c r="C119" s="144"/>
       <c r="D119" s="144"/>
@@ -8666,7 +8553,7 @@
         <v>7.9600000000000004E-2</v>
       </c>
       <c r="H119" s="159" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I119" s="148"/>
       <c r="J119" s="144"/>
@@ -8706,7 +8593,7 @@
       <c r="AR119" s="144"/>
       <c r="AS119" s="144"/>
     </row>
-    <row r="120" spans="2:45" s="139" customFormat="1">
+    <row r="120" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B120" s="137"/>
       <c r="C120" s="144"/>
       <c r="D120" s="144"/>
@@ -8751,7 +8638,7 @@
       <c r="AR120" s="144"/>
       <c r="AS120" s="144"/>
     </row>
-    <row r="121" spans="2:45" s="139" customFormat="1">
+    <row r="121" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B121" s="137"/>
       <c r="C121" s="144"/>
       <c r="D121" s="144"/>
@@ -8796,7 +8683,7 @@
       <c r="AR121" s="144"/>
       <c r="AS121" s="144"/>
     </row>
-    <row r="122" spans="2:45" s="139" customFormat="1">
+    <row r="122" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B122" s="137"/>
       <c r="C122" s="144"/>
       <c r="D122" s="144"/>
@@ -8841,7 +8728,7 @@
       <c r="AR122" s="144"/>
       <c r="AS122" s="144"/>
     </row>
-    <row r="123" spans="2:45" s="139" customFormat="1">
+    <row r="123" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B123" s="137"/>
       <c r="C123" s="144"/>
       <c r="D123" s="144"/>
@@ -8886,7 +8773,7 @@
       <c r="AR123" s="144"/>
       <c r="AS123" s="144"/>
     </row>
-    <row r="124" spans="2:45" s="139" customFormat="1">
+    <row r="124" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B124" s="137"/>
       <c r="C124" s="144"/>
       <c r="D124" s="144"/>
@@ -8931,7 +8818,7 @@
       <c r="AR124" s="144"/>
       <c r="AS124" s="144"/>
     </row>
-    <row r="125" spans="2:45" s="139" customFormat="1">
+    <row r="125" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B125" s="137"/>
       <c r="C125" s="144"/>
       <c r="D125" s="144"/>
@@ -8976,7 +8863,7 @@
       <c r="AR125" s="144"/>
       <c r="AS125" s="144"/>
     </row>
-    <row r="126" spans="2:45" s="139" customFormat="1">
+    <row r="126" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B126" s="137"/>
       <c r="C126" s="144"/>
       <c r="D126" s="144"/>
@@ -9021,7 +8908,7 @@
       <c r="AR126" s="144"/>
       <c r="AS126" s="144"/>
     </row>
-    <row r="127" spans="2:45" s="139" customFormat="1">
+    <row r="127" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B127" s="137"/>
       <c r="C127" s="144"/>
       <c r="D127" s="144"/>
@@ -9066,7 +8953,7 @@
       <c r="AR127" s="144"/>
       <c r="AS127" s="144"/>
     </row>
-    <row r="128" spans="2:45" s="139" customFormat="1">
+    <row r="128" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B128" s="137"/>
       <c r="C128" s="144"/>
       <c r="D128" s="144"/>
@@ -9111,7 +8998,7 @@
       <c r="AR128" s="144"/>
       <c r="AS128" s="144"/>
     </row>
-    <row r="129" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="129" spans="2:45" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B129" s="137"/>
       <c r="C129" s="144"/>
       <c r="D129" s="144"/>
@@ -9156,7 +9043,7 @@
       <c r="AR129" s="144"/>
       <c r="AS129" s="144"/>
     </row>
-    <row r="130" spans="2:45" s="135" customFormat="1">
+    <row r="130" spans="2:45" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B130" s="134"/>
       <c r="C130" s="134" t="s">
         <v>24</v>
@@ -9184,7 +9071,7 @@
       <c r="T130" s="134"/>
       <c r="U130" s="134"/>
     </row>
-    <row r="131" spans="2:45" s="139" customFormat="1">
+    <row r="131" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B131" s="136"/>
       <c r="C131" s="144"/>
       <c r="D131" s="144"/>
@@ -9210,7 +9097,7 @@
       <c r="X131" s="144"/>
       <c r="Y131" s="144"/>
     </row>
-    <row r="132" spans="2:45" s="139" customFormat="1">
+    <row r="132" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B132" s="136"/>
       <c r="C132" s="144" t="s">
         <v>51</v>
@@ -9238,7 +9125,7 @@
       <c r="X132" s="144"/>
       <c r="Y132" s="144"/>
     </row>
-    <row r="133" spans="2:45" s="139" customFormat="1">
+    <row r="133" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B133" s="136"/>
       <c r="C133" s="144"/>
       <c r="D133" s="144"/>
@@ -9264,7 +9151,7 @@
       <c r="X133" s="144"/>
       <c r="Y133" s="144"/>
     </row>
-    <row r="134" spans="2:45" s="139" customFormat="1">
+    <row r="134" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B134" s="136"/>
       <c r="C134" s="144"/>
       <c r="D134" s="144"/>
@@ -9290,7 +9177,7 @@
       <c r="X134" s="144"/>
       <c r="Y134" s="144"/>
     </row>
-    <row r="135" spans="2:45" s="139" customFormat="1">
+    <row r="135" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B135" s="136"/>
       <c r="C135" s="144"/>
       <c r="D135" s="144"/>
@@ -9316,7 +9203,7 @@
       <c r="X135" s="144"/>
       <c r="Y135" s="144"/>
     </row>
-    <row r="136" spans="2:45" s="139" customFormat="1" ht="18">
+    <row r="136" spans="2:45" s="139" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="B136" s="136"/>
       <c r="C136" s="144"/>
       <c r="D136" s="144">
@@ -9324,7 +9211,7 @@
       </c>
       <c r="F136" s="144"/>
       <c r="G136" s="139" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H136" s="153" t="s">
         <v>52</v>
@@ -9347,7 +9234,7 @@
       <c r="X136" s="144"/>
       <c r="Y136" s="144"/>
     </row>
-    <row r="137" spans="2:45" s="139" customFormat="1">
+    <row r="137" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B137" s="136"/>
       <c r="C137" s="144"/>
       <c r="D137" s="144"/>
@@ -9376,13 +9263,13 @@
       <c r="X137" s="144"/>
       <c r="Y137" s="144"/>
     </row>
-    <row r="138" spans="2:45" s="139" customFormat="1" ht="18">
+    <row r="138" spans="2:45" s="139" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="B138" s="136"/>
       <c r="C138" s="144"/>
       <c r="D138" s="144"/>
       <c r="F138" s="144"/>
       <c r="G138" s="139" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H138" s="153" t="s">
         <v>55</v>
@@ -9405,7 +9292,7 @@
       <c r="X138" s="144"/>
       <c r="Y138" s="144"/>
     </row>
-    <row r="139" spans="2:45" s="139" customFormat="1">
+    <row r="139" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B139" s="136"/>
       <c r="C139" s="144"/>
       <c r="D139" s="144"/>
@@ -9434,7 +9321,7 @@
       <c r="X139" s="144"/>
       <c r="Y139" s="144"/>
     </row>
-    <row r="140" spans="2:45" s="139" customFormat="1">
+    <row r="140" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B140" s="136"/>
       <c r="C140" s="144"/>
       <c r="D140" s="144"/>
@@ -9460,7 +9347,7 @@
       <c r="X140" s="144"/>
       <c r="Y140" s="144"/>
     </row>
-    <row r="141" spans="2:45" s="139" customFormat="1">
+    <row r="141" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B141" s="136"/>
       <c r="C141" s="144"/>
       <c r="D141" s="144"/>
@@ -9486,7 +9373,7 @@
       <c r="X141" s="144"/>
       <c r="Y141" s="144"/>
     </row>
-    <row r="142" spans="2:45" s="139" customFormat="1">
+    <row r="142" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B142" s="136"/>
       <c r="C142" s="144"/>
       <c r="D142" s="144"/>
@@ -9512,7 +9399,7 @@
       <c r="X142" s="144"/>
       <c r="Y142" s="144"/>
     </row>
-    <row r="143" spans="2:45" s="139" customFormat="1">
+    <row r="143" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B143" s="136"/>
       <c r="C143" s="144"/>
       <c r="D143" s="144"/>
@@ -9538,7 +9425,7 @@
       <c r="X143" s="144"/>
       <c r="Y143" s="144"/>
     </row>
-    <row r="144" spans="2:45" s="139" customFormat="1">
+    <row r="144" spans="2:45" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B144" s="136"/>
       <c r="C144" s="144"/>
       <c r="D144" s="144"/>
@@ -9564,7 +9451,7 @@
       <c r="X144" s="144"/>
       <c r="Y144" s="144"/>
     </row>
-    <row r="145" spans="2:25" s="139" customFormat="1">
+    <row r="145" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B145" s="136"/>
       <c r="C145" s="144"/>
       <c r="D145" s="144"/>
@@ -9590,7 +9477,7 @@
       <c r="X145" s="144"/>
       <c r="Y145" s="144"/>
     </row>
-    <row r="146" spans="2:25" s="139" customFormat="1">
+    <row r="146" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B146" s="136"/>
       <c r="C146" s="144"/>
       <c r="D146" s="144"/>
@@ -9616,7 +9503,7 @@
       <c r="X146" s="144"/>
       <c r="Y146" s="144"/>
     </row>
-    <row r="147" spans="2:25" s="139" customFormat="1">
+    <row r="147" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B147" s="136"/>
       <c r="C147" s="144"/>
       <c r="D147" s="144"/>
@@ -9642,7 +9529,7 @@
       <c r="X147" s="144"/>
       <c r="Y147" s="144"/>
     </row>
-    <row r="148" spans="2:25" s="139" customFormat="1">
+    <row r="148" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B148" s="136"/>
       <c r="C148" s="144"/>
       <c r="D148" s="144"/>
@@ -9668,7 +9555,7 @@
       <c r="X148" s="144"/>
       <c r="Y148" s="144"/>
     </row>
-    <row r="149" spans="2:25" s="139" customFormat="1">
+    <row r="149" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B149" s="136"/>
       <c r="C149" s="144"/>
       <c r="D149" s="144"/>
@@ -9694,7 +9581,7 @@
       <c r="X149" s="144"/>
       <c r="Y149" s="144"/>
     </row>
-    <row r="150" spans="2:25" s="139" customFormat="1">
+    <row r="150" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B150" s="136"/>
       <c r="C150" s="144"/>
       <c r="D150" s="144"/>
@@ -9720,7 +9607,7 @@
       <c r="X150" s="144"/>
       <c r="Y150" s="144"/>
     </row>
-    <row r="151" spans="2:25" s="139" customFormat="1">
+    <row r="151" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B151" s="136"/>
       <c r="C151" s="144"/>
       <c r="D151" s="144"/>
@@ -9746,7 +9633,7 @@
       <c r="X151" s="144"/>
       <c r="Y151" s="144"/>
     </row>
-    <row r="152" spans="2:25" s="139" customFormat="1">
+    <row r="152" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B152" s="136"/>
       <c r="C152" s="144"/>
       <c r="D152" s="144"/>
@@ -9772,7 +9659,7 @@
       <c r="X152" s="144"/>
       <c r="Y152" s="144"/>
     </row>
-    <row r="153" spans="2:25" s="139" customFormat="1">
+    <row r="153" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B153" s="136"/>
       <c r="C153" s="144"/>
       <c r="D153" s="144"/>
@@ -9798,7 +9685,7 @@
       <c r="X153" s="144"/>
       <c r="Y153" s="144"/>
     </row>
-    <row r="154" spans="2:25" s="139" customFormat="1">
+    <row r="154" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B154" s="136"/>
       <c r="C154" s="144"/>
       <c r="D154" s="144"/>
@@ -9824,7 +9711,7 @@
       <c r="X154" s="144"/>
       <c r="Y154" s="144"/>
     </row>
-    <row r="155" spans="2:25" s="139" customFormat="1">
+    <row r="155" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B155" s="136"/>
       <c r="C155" s="144"/>
       <c r="D155" s="144"/>
@@ -9850,7 +9737,7 @@
       <c r="X155" s="144"/>
       <c r="Y155" s="144"/>
     </row>
-    <row r="156" spans="2:25" s="139" customFormat="1">
+    <row r="156" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B156" s="136"/>
       <c r="C156" s="144"/>
       <c r="D156" s="144"/>
@@ -9876,106 +9763,106 @@
       <c r="X156" s="144"/>
       <c r="Y156" s="144"/>
     </row>
-    <row r="157" spans="2:25" s="139" customFormat="1">
+    <row r="157" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B157" s="136"/>
     </row>
-    <row r="158" spans="2:25" s="139" customFormat="1">
+    <row r="158" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B158" s="136"/>
     </row>
-    <row r="159" spans="2:25" s="139" customFormat="1">
+    <row r="159" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B159" s="136"/>
     </row>
-    <row r="160" spans="2:25" s="139" customFormat="1">
+    <row r="160" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B160" s="136"/>
     </row>
-    <row r="161" spans="2:2" s="139" customFormat="1">
+    <row r="161" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B161" s="136"/>
     </row>
-    <row r="162" spans="2:2" s="139" customFormat="1">
+    <row r="162" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B162" s="136"/>
     </row>
-    <row r="163" spans="2:2" s="139" customFormat="1">
+    <row r="163" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B163" s="136"/>
     </row>
-    <row r="164" spans="2:2" s="139" customFormat="1">
+    <row r="164" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B164" s="136"/>
     </row>
-    <row r="165" spans="2:2" s="139" customFormat="1">
+    <row r="165" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B165" s="136"/>
     </row>
-    <row r="166" spans="2:2" s="139" customFormat="1">
+    <row r="166" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B166" s="136"/>
     </row>
-    <row r="167" spans="2:2" s="139" customFormat="1">
+    <row r="167" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B167" s="136"/>
     </row>
-    <row r="168" spans="2:2" s="139" customFormat="1">
+    <row r="168" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B168" s="136"/>
     </row>
-    <row r="169" spans="2:2" s="139" customFormat="1">
+    <row r="169" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B169" s="136"/>
     </row>
-    <row r="170" spans="2:2" s="139" customFormat="1">
+    <row r="170" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B170" s="136"/>
     </row>
-    <row r="171" spans="2:2" s="139" customFormat="1">
+    <row r="171" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B171" s="136"/>
     </row>
-    <row r="172" spans="2:2" s="139" customFormat="1">
+    <row r="172" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B172" s="136"/>
     </row>
-    <row r="173" spans="2:2" s="139" customFormat="1">
+    <row r="173" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B173" s="136"/>
     </row>
-    <row r="174" spans="2:2" s="139" customFormat="1">
+    <row r="174" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B174" s="136"/>
     </row>
-    <row r="175" spans="2:2" s="139" customFormat="1">
+    <row r="175" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B175" s="136"/>
     </row>
-    <row r="176" spans="2:2" s="139" customFormat="1">
+    <row r="176" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B176" s="136"/>
     </row>
-    <row r="177" spans="2:25" s="139" customFormat="1">
+    <row r="177" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B177" s="136"/>
     </row>
-    <row r="178" spans="2:25" s="139" customFormat="1">
+    <row r="178" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B178" s="136"/>
     </row>
-    <row r="179" spans="2:25" s="139" customFormat="1">
+    <row r="179" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B179" s="136"/>
     </row>
-    <row r="180" spans="2:25" s="139" customFormat="1">
+    <row r="180" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B180" s="136"/>
     </row>
-    <row r="181" spans="2:25" s="139" customFormat="1">
+    <row r="181" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B181" s="136"/>
     </row>
-    <row r="182" spans="2:25" s="139" customFormat="1">
+    <row r="182" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B182" s="136"/>
     </row>
-    <row r="183" spans="2:25" s="139" customFormat="1">
+    <row r="183" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B183" s="136"/>
     </row>
-    <row r="184" spans="2:25" s="139" customFormat="1">
+    <row r="184" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B184" s="136"/>
     </row>
-    <row r="185" spans="2:25" s="139" customFormat="1">
+    <row r="185" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B185" s="136"/>
     </row>
-    <row r="186" spans="2:25" s="139" customFormat="1">
+    <row r="186" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B186" s="136"/>
     </row>
-    <row r="187" spans="2:25" s="139" customFormat="1">
+    <row r="187" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B187" s="136"/>
     </row>
-    <row r="188" spans="2:25" s="139" customFormat="1">
+    <row r="188" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B188" s="136"/>
     </row>
-    <row r="189" spans="2:25" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="189" spans="2:25" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="136"/>
     </row>
-    <row r="190" spans="2:25" s="135" customFormat="1">
+    <row r="190" spans="2:25" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B190" s="134"/>
       <c r="C190" s="134" t="s">
         <v>24</v>
@@ -10003,7 +9890,7 @@
       <c r="T190" s="134"/>
       <c r="U190" s="134"/>
     </row>
-    <row r="191" spans="2:25" s="139" customFormat="1">
+    <row r="191" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B191" s="136"/>
       <c r="C191" s="144"/>
       <c r="D191" s="144"/>
@@ -10029,7 +9916,7 @@
       <c r="X191" s="144"/>
       <c r="Y191" s="144"/>
     </row>
-    <row r="192" spans="2:25" s="139" customFormat="1">
+    <row r="192" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B192" s="136"/>
       <c r="C192" s="140" t="s">
         <v>57</v>
@@ -10057,7 +9944,7 @@
       <c r="X192" s="144"/>
       <c r="Y192" s="144"/>
     </row>
-    <row r="193" spans="2:25" s="139" customFormat="1">
+    <row r="193" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B193" s="136"/>
       <c r="C193" s="132"/>
       <c r="D193" s="144"/>
@@ -10083,7 +9970,7 @@
       <c r="X193" s="144"/>
       <c r="Y193" s="144"/>
     </row>
-    <row r="194" spans="2:25" s="139" customFormat="1">
+    <row r="194" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B194" s="136"/>
       <c r="C194" s="144"/>
       <c r="D194" s="139">
@@ -10111,7 +9998,7 @@
       <c r="X194" s="144"/>
       <c r="Y194" s="144"/>
     </row>
-    <row r="195" spans="2:25" s="139" customFormat="1">
+    <row r="195" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B195" s="136"/>
       <c r="C195" s="144"/>
       <c r="D195" s="144"/>
@@ -10137,7 +10024,7 @@
       <c r="X195" s="144"/>
       <c r="Y195" s="144"/>
     </row>
-    <row r="196" spans="2:25" s="139" customFormat="1">
+    <row r="196" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B196" s="136"/>
       <c r="C196" s="144"/>
       <c r="D196" s="144"/>
@@ -10161,7 +10048,7 @@
       <c r="X196" s="144"/>
       <c r="Y196" s="144"/>
     </row>
-    <row r="197" spans="2:25" s="139" customFormat="1">
+    <row r="197" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B197" s="136"/>
       <c r="C197" s="144"/>
       <c r="D197" s="144"/>
@@ -10186,7 +10073,7 @@
       <c r="X197" s="144"/>
       <c r="Y197" s="144"/>
     </row>
-    <row r="198" spans="2:25" s="139" customFormat="1">
+    <row r="198" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B198" s="136"/>
       <c r="C198" s="144"/>
       <c r="D198" s="144"/>
@@ -10210,7 +10097,7 @@
       <c r="X198" s="144"/>
       <c r="Y198" s="144"/>
     </row>
-    <row r="199" spans="2:25" s="139" customFormat="1">
+    <row r="199" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B199" s="136"/>
       <c r="C199" s="144"/>
       <c r="D199" s="144"/>
@@ -10235,7 +10122,7 @@
       <c r="X199" s="144"/>
       <c r="Y199" s="144"/>
     </row>
-    <row r="200" spans="2:25" s="139" customFormat="1">
+    <row r="200" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B200" s="136"/>
       <c r="C200" s="144"/>
       <c r="D200" s="144"/>
@@ -10261,7 +10148,7 @@
       <c r="X200" s="144"/>
       <c r="Y200" s="144"/>
     </row>
-    <row r="201" spans="2:25" s="139" customFormat="1">
+    <row r="201" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B201" s="136"/>
       <c r="C201" s="144"/>
       <c r="D201" s="144"/>
@@ -10287,7 +10174,7 @@
       <c r="X201" s="144"/>
       <c r="Y201" s="144"/>
     </row>
-    <row r="202" spans="2:25" s="139" customFormat="1">
+    <row r="202" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B202" s="136"/>
       <c r="C202" s="144"/>
       <c r="D202" s="144"/>
@@ -10313,7 +10200,7 @@
       <c r="X202" s="144"/>
       <c r="Y202" s="144"/>
     </row>
-    <row r="203" spans="2:25" s="139" customFormat="1">
+    <row r="203" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B203" s="136"/>
       <c r="C203" s="144"/>
       <c r="D203" s="144"/>
@@ -10339,7 +10226,7 @@
       <c r="X203" s="144"/>
       <c r="Y203" s="144"/>
     </row>
-    <row r="204" spans="2:25" s="139" customFormat="1">
+    <row r="204" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B204" s="136"/>
       <c r="C204" s="144"/>
       <c r="D204" s="144"/>
@@ -10365,7 +10252,7 @@
       <c r="X204" s="144"/>
       <c r="Y204" s="144"/>
     </row>
-    <row r="205" spans="2:25" s="139" customFormat="1">
+    <row r="205" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B205" s="136"/>
       <c r="C205" s="144"/>
       <c r="D205" s="144"/>
@@ -10391,7 +10278,7 @@
       <c r="X205" s="144"/>
       <c r="Y205" s="144"/>
     </row>
-    <row r="206" spans="2:25" s="139" customFormat="1">
+    <row r="206" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B206" s="136"/>
       <c r="C206" s="144"/>
       <c r="D206" s="144"/>
@@ -10417,7 +10304,7 @@
       <c r="X206" s="144"/>
       <c r="Y206" s="144"/>
     </row>
-    <row r="207" spans="2:25" s="139" customFormat="1">
+    <row r="207" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B207" s="136"/>
       <c r="C207" s="144"/>
       <c r="D207" s="144"/>
@@ -10443,7 +10330,7 @@
       <c r="X207" s="144"/>
       <c r="Y207" s="144"/>
     </row>
-    <row r="208" spans="2:25" s="139" customFormat="1">
+    <row r="208" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B208" s="136"/>
       <c r="C208" s="144"/>
       <c r="D208" s="144"/>
@@ -10469,7 +10356,7 @@
       <c r="X208" s="144"/>
       <c r="Y208" s="144"/>
     </row>
-    <row r="209" spans="2:25" s="139" customFormat="1">
+    <row r="209" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B209" s="136"/>
       <c r="C209" s="144"/>
       <c r="D209" s="144"/>
@@ -10495,7 +10382,7 @@
       <c r="X209" s="144"/>
       <c r="Y209" s="144"/>
     </row>
-    <row r="210" spans="2:25" s="139" customFormat="1">
+    <row r="210" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B210" s="136"/>
       <c r="C210" s="144"/>
       <c r="D210" s="144"/>
@@ -10521,7 +10408,7 @@
       <c r="X210" s="144"/>
       <c r="Y210" s="144"/>
     </row>
-    <row r="211" spans="2:25" s="139" customFormat="1">
+    <row r="211" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B211" s="136"/>
       <c r="C211" s="144"/>
       <c r="D211" s="144"/>
@@ -10547,7 +10434,7 @@
       <c r="X211" s="144"/>
       <c r="Y211" s="144"/>
     </row>
-    <row r="212" spans="2:25" s="139" customFormat="1">
+    <row r="212" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B212" s="136"/>
       <c r="C212" s="144"/>
       <c r="D212" s="144"/>
@@ -10573,7 +10460,7 @@
       <c r="X212" s="144"/>
       <c r="Y212" s="144"/>
     </row>
-    <row r="213" spans="2:25" s="139" customFormat="1">
+    <row r="213" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B213" s="136"/>
       <c r="C213" s="144"/>
       <c r="D213" s="144"/>
@@ -10599,7 +10486,7 @@
       <c r="X213" s="144"/>
       <c r="Y213" s="144"/>
     </row>
-    <row r="214" spans="2:25" s="139" customFormat="1">
+    <row r="214" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B214" s="136"/>
       <c r="C214" s="144"/>
       <c r="D214" s="144"/>
@@ -10625,7 +10512,7 @@
       <c r="X214" s="144"/>
       <c r="Y214" s="144"/>
     </row>
-    <row r="215" spans="2:25" s="139" customFormat="1">
+    <row r="215" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B215" s="136"/>
       <c r="C215" s="144"/>
       <c r="D215" s="144"/>
@@ -10651,7 +10538,7 @@
       <c r="X215" s="144"/>
       <c r="Y215" s="144"/>
     </row>
-    <row r="216" spans="2:25" s="139" customFormat="1">
+    <row r="216" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B216" s="136"/>
       <c r="C216" s="144"/>
       <c r="D216" s="144"/>
@@ -10677,364 +10564,364 @@
       <c r="X216" s="144"/>
       <c r="Y216" s="144"/>
     </row>
-    <row r="217" spans="2:25" s="139" customFormat="1">
+    <row r="217" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B217" s="136"/>
     </row>
-    <row r="218" spans="2:25" s="139" customFormat="1">
+    <row r="218" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B218" s="136"/>
     </row>
-    <row r="219" spans="2:25" s="139" customFormat="1">
+    <row r="219" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B219" s="136"/>
     </row>
-    <row r="220" spans="2:25" s="139" customFormat="1">
+    <row r="220" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B220" s="136"/>
     </row>
-    <row r="221" spans="2:25" s="139" customFormat="1">
+    <row r="221" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B221" s="136"/>
       <c r="D221" s="139">
         <v>111</v>
       </c>
     </row>
-    <row r="222" spans="2:25" s="139" customFormat="1">
+    <row r="222" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B222" s="136"/>
     </row>
-    <row r="223" spans="2:25" s="139" customFormat="1">
+    <row r="223" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B223" s="136"/>
     </row>
-    <row r="224" spans="2:25" s="139" customFormat="1">
+    <row r="224" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B224" s="136"/>
     </row>
-    <row r="225" spans="2:2" s="139" customFormat="1">
+    <row r="225" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B225" s="136"/>
     </row>
-    <row r="226" spans="2:2" s="139" customFormat="1">
+    <row r="226" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B226" s="136"/>
     </row>
-    <row r="227" spans="2:2" s="139" customFormat="1">
+    <row r="227" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B227" s="136"/>
     </row>
-    <row r="228" spans="2:2" s="139" customFormat="1">
+    <row r="228" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B228" s="136"/>
     </row>
-    <row r="229" spans="2:2" s="139" customFormat="1">
+    <row r="229" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B229" s="136"/>
     </row>
-    <row r="230" spans="2:2" s="139" customFormat="1">
+    <row r="230" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B230" s="136"/>
     </row>
-    <row r="231" spans="2:2" s="139" customFormat="1">
+    <row r="231" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B231" s="136"/>
     </row>
-    <row r="232" spans="2:2" s="139" customFormat="1">
+    <row r="232" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B232" s="136"/>
     </row>
-    <row r="233" spans="2:2" s="139" customFormat="1">
+    <row r="233" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B233" s="136"/>
     </row>
-    <row r="234" spans="2:2" s="139" customFormat="1">
+    <row r="234" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B234" s="136"/>
     </row>
-    <row r="235" spans="2:2" s="139" customFormat="1">
+    <row r="235" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B235" s="136"/>
     </row>
-    <row r="236" spans="2:2" s="139" customFormat="1">
+    <row r="236" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B236" s="136"/>
     </row>
-    <row r="237" spans="2:2" s="139" customFormat="1">
+    <row r="237" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B237" s="136"/>
     </row>
-    <row r="238" spans="2:2" s="139" customFormat="1">
+    <row r="238" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B238" s="136"/>
     </row>
-    <row r="239" spans="2:2" s="139" customFormat="1">
+    <row r="239" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B239" s="136"/>
     </row>
-    <row r="240" spans="2:2" s="139" customFormat="1">
+    <row r="240" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B240" s="136"/>
     </row>
-    <row r="241" spans="2:4" s="139" customFormat="1">
+    <row r="241" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B241" s="136"/>
     </row>
-    <row r="242" spans="2:4" s="139" customFormat="1">
+    <row r="242" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B242" s="136"/>
     </row>
-    <row r="243" spans="2:4" s="139" customFormat="1">
+    <row r="243" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B243" s="136"/>
     </row>
-    <row r="244" spans="2:4" s="139" customFormat="1">
+    <row r="244" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B244" s="136"/>
       <c r="D244" s="139">
         <v>112</v>
       </c>
     </row>
-    <row r="245" spans="2:4" s="139" customFormat="1">
+    <row r="245" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B245" s="136"/>
     </row>
-    <row r="246" spans="2:4" s="139" customFormat="1">
+    <row r="246" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B246" s="136"/>
     </row>
-    <row r="247" spans="2:4" s="139" customFormat="1">
+    <row r="247" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B247" s="136"/>
     </row>
-    <row r="248" spans="2:4" s="139" customFormat="1">
+    <row r="248" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B248" s="136"/>
     </row>
-    <row r="249" spans="2:4" s="139" customFormat="1">
+    <row r="249" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B249" s="136"/>
     </row>
-    <row r="250" spans="2:4" s="139" customFormat="1">
+    <row r="250" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B250" s="136"/>
     </row>
-    <row r="251" spans="2:4" s="139" customFormat="1">
+    <row r="251" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B251" s="136"/>
     </row>
-    <row r="252" spans="2:4" s="139" customFormat="1">
+    <row r="252" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B252" s="136"/>
     </row>
-    <row r="253" spans="2:4" s="139" customFormat="1">
+    <row r="253" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B253" s="136"/>
     </row>
-    <row r="254" spans="2:4" s="139" customFormat="1">
+    <row r="254" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B254" s="136"/>
     </row>
-    <row r="255" spans="2:4" s="139" customFormat="1">
+    <row r="255" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B255" s="136"/>
     </row>
-    <row r="256" spans="2:4" s="139" customFormat="1">
+    <row r="256" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B256" s="136"/>
     </row>
-    <row r="257" spans="2:4" s="139" customFormat="1">
+    <row r="257" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B257" s="136"/>
     </row>
-    <row r="258" spans="2:4" s="139" customFormat="1">
+    <row r="258" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B258" s="136"/>
     </row>
-    <row r="259" spans="2:4" s="139" customFormat="1">
+    <row r="259" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B259" s="136"/>
     </row>
-    <row r="260" spans="2:4" s="139" customFormat="1">
+    <row r="260" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B260" s="136"/>
     </row>
-    <row r="261" spans="2:4" s="139" customFormat="1">
+    <row r="261" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B261" s="136"/>
     </row>
-    <row r="262" spans="2:4" s="139" customFormat="1">
+    <row r="262" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B262" s="136"/>
     </row>
-    <row r="263" spans="2:4" s="139" customFormat="1">
+    <row r="263" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B263" s="136"/>
     </row>
-    <row r="264" spans="2:4" s="139" customFormat="1">
+    <row r="264" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B264" s="136"/>
     </row>
-    <row r="265" spans="2:4" s="139" customFormat="1">
+    <row r="265" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B265" s="136"/>
     </row>
-    <row r="266" spans="2:4" s="139" customFormat="1">
+    <row r="266" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B266" s="136"/>
     </row>
-    <row r="267" spans="2:4" s="139" customFormat="1">
+    <row r="267" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B267" s="136"/>
     </row>
-    <row r="268" spans="2:4" s="139" customFormat="1">
+    <row r="268" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B268" s="136"/>
       <c r="D268" s="139">
         <v>113</v>
       </c>
     </row>
-    <row r="269" spans="2:4" s="139" customFormat="1">
+    <row r="269" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B269" s="136"/>
     </row>
-    <row r="270" spans="2:4" s="139" customFormat="1">
+    <row r="270" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B270" s="136"/>
     </row>
-    <row r="271" spans="2:4" s="139" customFormat="1">
+    <row r="271" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B271" s="136"/>
     </row>
-    <row r="272" spans="2:4" s="139" customFormat="1">
+    <row r="272" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B272" s="136"/>
     </row>
-    <row r="273" spans="2:2" s="139" customFormat="1">
+    <row r="273" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B273" s="136"/>
     </row>
-    <row r="274" spans="2:2" s="139" customFormat="1">
+    <row r="274" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B274" s="136"/>
     </row>
-    <row r="275" spans="2:2" s="139" customFormat="1">
+    <row r="275" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B275" s="136"/>
     </row>
-    <row r="276" spans="2:2" s="139" customFormat="1">
+    <row r="276" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B276" s="136"/>
     </row>
-    <row r="277" spans="2:2" s="139" customFormat="1">
+    <row r="277" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B277" s="136"/>
     </row>
-    <row r="278" spans="2:2" s="139" customFormat="1">
+    <row r="278" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B278" s="136"/>
     </row>
-    <row r="279" spans="2:2" s="139" customFormat="1">
+    <row r="279" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B279" s="136"/>
     </row>
-    <row r="280" spans="2:2" s="139" customFormat="1">
+    <row r="280" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B280" s="136"/>
     </row>
-    <row r="281" spans="2:2" s="139" customFormat="1">
+    <row r="281" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B281" s="136"/>
     </row>
-    <row r="282" spans="2:2" s="139" customFormat="1">
+    <row r="282" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B282" s="136"/>
     </row>
-    <row r="283" spans="2:2" s="139" customFormat="1">
+    <row r="283" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B283" s="136"/>
     </row>
-    <row r="284" spans="2:2" s="139" customFormat="1">
+    <row r="284" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B284" s="136"/>
     </row>
-    <row r="285" spans="2:2" s="139" customFormat="1">
+    <row r="285" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B285" s="136"/>
     </row>
-    <row r="286" spans="2:2" s="139" customFormat="1">
+    <row r="286" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B286" s="136"/>
     </row>
-    <row r="287" spans="2:2" s="139" customFormat="1">
+    <row r="287" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B287" s="136"/>
     </row>
-    <row r="288" spans="2:2" s="139" customFormat="1">
+    <row r="288" spans="2:2" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B288" s="136"/>
     </row>
-    <row r="289" spans="2:4" s="139" customFormat="1">
+    <row r="289" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B289" s="136"/>
     </row>
-    <row r="290" spans="2:4" s="139" customFormat="1">
+    <row r="290" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B290" s="136"/>
     </row>
-    <row r="291" spans="2:4" s="139" customFormat="1">
+    <row r="291" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B291" s="136"/>
     </row>
-    <row r="292" spans="2:4" s="139" customFormat="1">
+    <row r="292" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B292" s="136"/>
     </row>
-    <row r="293" spans="2:4" s="139" customFormat="1">
+    <row r="293" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B293" s="136"/>
     </row>
-    <row r="294" spans="2:4" s="139" customFormat="1">
+    <row r="294" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B294" s="136"/>
       <c r="D294" s="139">
         <v>114</v>
       </c>
     </row>
-    <row r="295" spans="2:4" s="139" customFormat="1">
+    <row r="295" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B295" s="136"/>
     </row>
-    <row r="296" spans="2:4" s="139" customFormat="1">
+    <row r="296" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B296" s="136"/>
     </row>
-    <row r="297" spans="2:4" s="139" customFormat="1">
+    <row r="297" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B297" s="136"/>
     </row>
-    <row r="298" spans="2:4" s="139" customFormat="1">
+    <row r="298" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B298" s="136"/>
     </row>
-    <row r="299" spans="2:4" s="139" customFormat="1">
+    <row r="299" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B299" s="136"/>
     </row>
-    <row r="300" spans="2:4" s="139" customFormat="1">
+    <row r="300" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B300" s="136"/>
     </row>
-    <row r="301" spans="2:4" s="139" customFormat="1">
+    <row r="301" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B301" s="136"/>
     </row>
-    <row r="302" spans="2:4" s="139" customFormat="1">
+    <row r="302" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B302" s="136"/>
     </row>
-    <row r="303" spans="2:4" s="139" customFormat="1">
+    <row r="303" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B303" s="136"/>
     </row>
-    <row r="304" spans="2:4" s="139" customFormat="1">
+    <row r="304" spans="2:4" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B304" s="136"/>
     </row>
-    <row r="305" spans="2:7" s="139" customFormat="1">
+    <row r="305" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B305" s="136"/>
       <c r="G305" s="139" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="306" spans="2:7" s="139" customFormat="1">
+    <row r="306" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B306" s="136"/>
       <c r="G306" s="139" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="307" spans="2:7" s="139" customFormat="1">
+    <row r="307" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B307" s="136"/>
       <c r="G307" s="139" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="308" spans="2:7" s="139" customFormat="1">
+    <row r="308" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B308" s="136"/>
     </row>
-    <row r="309" spans="2:7" s="139" customFormat="1">
+    <row r="309" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B309" s="136"/>
     </row>
-    <row r="310" spans="2:7" s="139" customFormat="1">
+    <row r="310" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B310" s="136"/>
     </row>
-    <row r="311" spans="2:7" s="139" customFormat="1">
+    <row r="311" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B311" s="136"/>
     </row>
-    <row r="312" spans="2:7" s="139" customFormat="1">
+    <row r="312" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B312" s="136"/>
     </row>
-    <row r="313" spans="2:7" s="139" customFormat="1">
+    <row r="313" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B313" s="136"/>
     </row>
-    <row r="314" spans="2:7" s="139" customFormat="1">
+    <row r="314" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B314" s="136"/>
     </row>
-    <row r="315" spans="2:7" s="139" customFormat="1">
+    <row r="315" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B315" s="136"/>
     </row>
-    <row r="316" spans="2:7" s="139" customFormat="1">
+    <row r="316" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B316" s="136"/>
     </row>
-    <row r="317" spans="2:7" s="139" customFormat="1">
+    <row r="317" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B317" s="136"/>
     </row>
-    <row r="318" spans="2:7" s="139" customFormat="1">
+    <row r="318" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B318" s="136"/>
     </row>
-    <row r="319" spans="2:7" s="139" customFormat="1">
+    <row r="319" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B319" s="136"/>
     </row>
-    <row r="320" spans="2:7" s="139" customFormat="1">
+    <row r="320" spans="2:7" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B320" s="136"/>
     </row>
-    <row r="321" spans="2:25" s="139" customFormat="1">
+    <row r="321" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B321" s="136"/>
     </row>
-    <row r="322" spans="2:25" s="139" customFormat="1">
+    <row r="322" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B322" s="136"/>
     </row>
-    <row r="323" spans="2:25" s="139" customFormat="1">
+    <row r="323" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B323" s="136"/>
     </row>
-    <row r="324" spans="2:25" s="139" customFormat="1">
+    <row r="324" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B324" s="136"/>
     </row>
-    <row r="325" spans="2:25" s="139" customFormat="1">
+    <row r="325" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B325" s="136"/>
     </row>
-    <row r="326" spans="2:25" s="139" customFormat="1">
+    <row r="326" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B326" s="136"/>
     </row>
-    <row r="327" spans="2:25" s="139" customFormat="1">
+    <row r="327" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B327" s="136"/>
     </row>
-    <row r="328" spans="2:25" s="139" customFormat="1" ht="17" thickBot="1">
+    <row r="328" spans="2:25" s="139" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B328" s="136"/>
     </row>
-    <row r="329" spans="2:25" s="135" customFormat="1">
+    <row r="329" spans="2:25" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B329" s="134"/>
       <c r="C329" s="134" t="s">
         <v>24</v>
@@ -11062,7 +10949,7 @@
       <c r="T329" s="134"/>
       <c r="U329" s="134"/>
     </row>
-    <row r="330" spans="2:25" s="139" customFormat="1">
+    <row r="330" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B330" s="136"/>
       <c r="C330" s="138"/>
       <c r="D330" s="144"/>
@@ -11088,7 +10975,7 @@
       <c r="X330" s="144"/>
       <c r="Y330" s="144"/>
     </row>
-    <row r="331" spans="2:25" s="139" customFormat="1">
+    <row r="331" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B331" s="136"/>
       <c r="C331" s="152" t="s">
         <v>61</v>
@@ -11116,7 +11003,7 @@
       <c r="X331" s="144"/>
       <c r="Y331" s="144"/>
     </row>
-    <row r="332" spans="2:25" s="139" customFormat="1">
+    <row r="332" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B332" s="136"/>
       <c r="C332" s="144"/>
       <c r="D332" s="144"/>
@@ -11142,7 +11029,7 @@
       <c r="X332" s="144"/>
       <c r="Y332" s="144"/>
     </row>
-    <row r="333" spans="2:25" s="139" customFormat="1">
+    <row r="333" spans="2:25" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B333" s="136"/>
       <c r="C333" s="144"/>
       <c r="D333" s="144"/>
@@ -11168,15 +11055,15 @@
       <c r="X333" s="144"/>
       <c r="Y333" s="144"/>
     </row>
-    <row r="335" spans="2:25">
+    <row r="335" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D335" s="132">
         <v>12</v>
       </c>
     </row>
-    <row r="340" spans="4:11">
+    <row r="340" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E340" s="141"/>
     </row>
-    <row r="341" spans="4:11">
+    <row r="341" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E341" s="144"/>
       <c r="F341" s="144"/>
       <c r="G341" s="144"/>
@@ -11185,7 +11072,7 @@
       <c r="J341" s="144"/>
       <c r="K341" s="144"/>
     </row>
-    <row r="342" spans="4:11">
+    <row r="342" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E342" s="144"/>
       <c r="F342" s="144"/>
       <c r="G342" s="144"/>
@@ -11194,7 +11081,7 @@
       <c r="J342" s="144"/>
       <c r="K342" s="144"/>
     </row>
-    <row r="343" spans="4:11">
+    <row r="343" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E343" s="144"/>
       <c r="F343" s="144"/>
       <c r="G343" s="144"/>
@@ -11203,7 +11090,7 @@
       <c r="J343" s="144"/>
       <c r="K343" s="144"/>
     </row>
-    <row r="344" spans="4:11">
+    <row r="344" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D344" s="144"/>
       <c r="E344" s="144"/>
       <c r="F344" s="144"/>
@@ -11213,7 +11100,7 @@
       <c r="J344" s="144"/>
       <c r="K344" s="144"/>
     </row>
-    <row r="345" spans="4:11">
+    <row r="345" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D345" s="144"/>
       <c r="E345" s="144"/>
       <c r="F345" s="144"/>
@@ -11223,7 +11110,7 @@
       <c r="J345" s="144"/>
       <c r="K345" s="144"/>
     </row>
-    <row r="346" spans="4:11">
+    <row r="346" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D346" s="144"/>
       <c r="E346" s="144"/>
       <c r="F346" s="144"/>
@@ -11233,7 +11120,7 @@
       <c r="J346" s="144"/>
       <c r="K346" s="144"/>
     </row>
-    <row r="347" spans="4:11">
+    <row r="347" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D347" s="144"/>
       <c r="E347" s="144"/>
       <c r="F347" s="144"/>
@@ -11242,7 +11129,7 @@
       <c r="I347" s="144"/>
       <c r="J347" s="144"/>
     </row>
-    <row r="348" spans="4:11">
+    <row r="348" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D348" s="144"/>
       <c r="E348" s="144"/>
       <c r="F348" s="144"/>
@@ -11251,7 +11138,7 @@
       <c r="I348" s="144"/>
       <c r="J348" s="144"/>
     </row>
-    <row r="349" spans="4:11">
+    <row r="349" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D349" s="144"/>
       <c r="E349" s="144"/>
       <c r="F349" s="144"/>
@@ -11261,7 +11148,7 @@
       <c r="J349" s="144"/>
       <c r="K349" s="144"/>
     </row>
-    <row r="350" spans="4:11">
+    <row r="350" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E350" s="144"/>
       <c r="F350" s="144"/>
       <c r="G350" s="144"/>
@@ -11270,7 +11157,7 @@
       <c r="J350" s="144"/>
       <c r="K350" s="144"/>
     </row>
-    <row r="351" spans="4:11">
+    <row r="351" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E351" s="144"/>
       <c r="F351" s="144"/>
       <c r="G351" s="144"/>
@@ -11279,7 +11166,7 @@
       <c r="J351" s="144"/>
       <c r="K351" s="144"/>
     </row>
-    <row r="352" spans="4:11">
+    <row r="352" spans="4:11" x14ac:dyDescent="0.2">
       <c r="E352" s="144"/>
       <c r="F352" s="144"/>
       <c r="G352" s="144"/>
@@ -11288,7 +11175,7 @@
       <c r="J352" s="144"/>
       <c r="K352" s="144"/>
     </row>
-    <row r="353" spans="5:11">
+    <row r="353" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E353" s="144"/>
       <c r="F353" s="144"/>
       <c r="G353" s="144"/>
@@ -11297,7 +11184,7 @@
       <c r="J353" s="144"/>
       <c r="K353" s="144"/>
     </row>
-    <row r="354" spans="5:11">
+    <row r="354" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E354" s="144"/>
       <c r="F354" s="144"/>
       <c r="G354" s="144"/>
@@ -11306,7 +11193,7 @@
       <c r="J354" s="144"/>
       <c r="K354" s="144"/>
     </row>
-    <row r="357" spans="5:11">
+    <row r="357" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E357" s="142"/>
       <c r="F357" s="143"/>
       <c r="G357" s="143"/>
@@ -11315,7 +11202,7 @@
       <c r="J357" s="143"/>
       <c r="K357" s="143"/>
     </row>
-    <row r="358" spans="5:11">
+    <row r="358" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E358" s="144"/>
       <c r="F358" s="144"/>
       <c r="G358" s="144"/>
@@ -11324,7 +11211,7 @@
       <c r="J358" s="144"/>
       <c r="K358" s="144"/>
     </row>
-    <row r="359" spans="5:11">
+    <row r="359" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E359" s="144"/>
       <c r="F359" s="144"/>
       <c r="G359" s="144"/>
@@ -11333,7 +11220,7 @@
       <c r="J359" s="144"/>
       <c r="K359" s="144"/>
     </row>
-    <row r="360" spans="5:11">
+    <row r="360" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E360" s="144"/>
       <c r="F360" s="144"/>
       <c r="G360" s="144"/>
@@ -11342,7 +11229,7 @@
       <c r="J360" s="144"/>
       <c r="K360" s="144"/>
     </row>
-    <row r="361" spans="5:11">
+    <row r="361" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E361" s="144"/>
       <c r="F361" s="144"/>
       <c r="G361" s="144"/>
@@ -11351,7 +11238,7 @@
       <c r="J361" s="144"/>
       <c r="K361" s="144"/>
     </row>
-    <row r="362" spans="5:11">
+    <row r="362" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E362" s="144"/>
       <c r="F362" s="144"/>
       <c r="G362" s="144"/>
@@ -11360,7 +11247,7 @@
       <c r="J362" s="144"/>
       <c r="K362" s="144"/>
     </row>
-    <row r="363" spans="5:11">
+    <row r="363" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E363" s="144"/>
       <c r="F363" s="144"/>
       <c r="G363" s="144"/>
@@ -11369,7 +11256,7 @@
       <c r="J363" s="144"/>
       <c r="K363" s="144"/>
     </row>
-    <row r="364" spans="5:11">
+    <row r="364" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E364" s="144"/>
       <c r="F364" s="144"/>
       <c r="G364" s="144"/>
@@ -11378,7 +11265,7 @@
       <c r="J364" s="144"/>
       <c r="K364" s="143"/>
     </row>
-    <row r="365" spans="5:11">
+    <row r="365" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E365" s="144"/>
       <c r="F365" s="144"/>
       <c r="G365" s="144"/>
@@ -11387,7 +11274,7 @@
       <c r="J365" s="144"/>
       <c r="K365" s="143"/>
     </row>
-    <row r="366" spans="5:11">
+    <row r="366" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E366" s="144"/>
       <c r="F366" s="144"/>
       <c r="G366" s="144"/>
@@ -11396,7 +11283,7 @@
       <c r="J366" s="144"/>
       <c r="K366" s="144"/>
     </row>
-    <row r="367" spans="5:11">
+    <row r="367" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E367" s="144"/>
       <c r="F367" s="144"/>
       <c r="G367" s="144"/>
@@ -11405,7 +11292,7 @@
       <c r="J367" s="144"/>
       <c r="K367" s="144"/>
     </row>
-    <row r="368" spans="5:11">
+    <row r="368" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E368" s="144"/>
       <c r="F368" s="144"/>
       <c r="G368" s="144"/>
@@ -11414,7 +11301,7 @@
       <c r="J368" s="144"/>
       <c r="K368" s="144"/>
     </row>
-    <row r="369" spans="5:11">
+    <row r="369" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E369" s="144"/>
       <c r="F369" s="144"/>
       <c r="G369" s="144"/>
@@ -11423,7 +11310,7 @@
       <c r="J369" s="144"/>
       <c r="K369" s="144"/>
     </row>
-    <row r="370" spans="5:11">
+    <row r="370" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E370" s="144"/>
       <c r="F370" s="144"/>
       <c r="G370" s="144"/>
@@ -11432,7 +11319,7 @@
       <c r="J370" s="144"/>
       <c r="K370" s="144"/>
     </row>
-    <row r="371" spans="5:11">
+    <row r="371" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E371" s="144"/>
       <c r="F371" s="144"/>
       <c r="G371" s="144"/>
@@ -11441,8 +11328,8 @@
       <c r="J371" s="144"/>
       <c r="K371" s="144"/>
     </row>
-    <row r="389" s="139" customFormat="1"/>
-    <row r="390" s="139" customFormat="1"/>
+    <row r="389" s="139" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="390" s="139" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G52:I52"/>
@@ -11455,10 +11342,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>